<commit_message>
HumModRepository - Redoing the Web content to include pages describing normal values (note that all of this is used in model scaling).
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Organ Mass" sheetId="4" r:id="rId1"/>
     <sheet name="Gender" sheetId="5" r:id="rId2"/>
     <sheet name="Blood Pressures" sheetId="6" r:id="rId3"/>
-    <sheet name="Blood Flow" sheetId="7" r:id="rId4"/>
+    <sheet name="Organ Blood Flow" sheetId="7" r:id="rId4"/>
     <sheet name="Mass" sheetId="1" r:id="rId5"/>
     <sheet name="Calories" sheetId="2" r:id="rId6"/>
     <sheet name="Vascular Conductance" sheetId="3" r:id="rId7"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="105">
   <si>
     <t>Bone</t>
   </si>
@@ -308,16 +308,44 @@
   </si>
   <si>
     <t>Cardiac Output</t>
+  </si>
+  <si>
+    <t>Organ - Male</t>
+  </si>
+  <si>
+    <t>Adipose</t>
+  </si>
+  <si>
+    <t>Adrenal</t>
+  </si>
+  <si>
+    <t>Lung</t>
+  </si>
+  <si>
+    <t>Organ - Female</t>
+  </si>
+  <si>
+    <t>% Cardiac Output</t>
+  </si>
+  <si>
+    <t>Blood Flow</t>
+  </si>
+  <si>
+    <t>Blood Flow (/G)</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -348,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -358,6 +386,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,6 +1413,189 @@
       <c r="D20" s="1">
         <f>D18+D19</f>
         <v>60450</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22">
+        <v>0.47</v>
+      </c>
+      <c r="C22" s="1">
+        <f>10 * B22 * C2</f>
+        <v>284.11499999999995</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23">
+        <v>0.17</v>
+      </c>
+      <c r="C23" s="1">
+        <f>B23 * C22</f>
+        <v>48.299549999999996</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24">
+        <f>1-B23</f>
+        <v>0.83</v>
+      </c>
+      <c r="C24" s="1">
+        <f>B24 * C22</f>
+        <v>235.81544999999994</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26">
+        <v>40</v>
+      </c>
+      <c r="C26" s="1">
+        <f>10*B26*C2</f>
+        <v>24180</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27">
+        <v>0.12</v>
+      </c>
+      <c r="C27" s="1">
+        <f>C26*B27</f>
+        <v>2901.6</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28">
+        <f>1-B27</f>
+        <v>0.88</v>
+      </c>
+      <c r="C28" s="1">
+        <f>C26*B28</f>
+        <v>21278.400000000001</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30">
+        <v>0.02</v>
+      </c>
+      <c r="D30" s="5">
+        <f>10*B30*C2</f>
+        <v>12.090000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31">
+        <v>0.21</v>
+      </c>
+      <c r="D31" s="5">
+        <f>10*B31*C2</f>
+        <v>126.94500000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32">
+        <v>0.91</v>
+      </c>
+      <c r="D32" s="5">
+        <f>10*B32*C2</f>
+        <v>550.09500000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33">
+        <v>0.53</v>
+      </c>
+      <c r="D33" s="5">
+        <f>10*B33*C2</f>
+        <v>320.38500000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34">
+        <v>0.76</v>
+      </c>
+      <c r="D34" s="5">
+        <f>10*B34*C2</f>
+        <v>459.42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D35" s="5">
+        <f>10*B35*C2</f>
+        <v>84.63000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36">
+        <v>0.26</v>
+      </c>
+      <c r="D36" s="5">
+        <f>10*B36*C2</f>
+        <v>157.17000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37">
+        <v>0.03</v>
+      </c>
+      <c r="D37" s="5">
+        <f>10*B37*C2</f>
+        <v>18.135000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1427,7 +1639,7 @@
         <v>97</v>
       </c>
       <c r="C2" s="5">
-        <f>0.1333*B2</f>
+        <f t="shared" ref="C2:C9" si="0">0.1333*B2</f>
         <v>12.930099999999999</v>
       </c>
       <c r="D2">
@@ -1443,7 +1655,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="5">
-        <f>0.1333*B3</f>
+        <f t="shared" si="0"/>
         <v>1.333</v>
       </c>
       <c r="D3">
@@ -1459,7 +1671,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="5">
-        <f>0.1333*B4</f>
+        <f t="shared" si="0"/>
         <v>1.0664</v>
       </c>
       <c r="D4">
@@ -1475,7 +1687,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5">
-        <f>0.1333*B5</f>
+        <f t="shared" si="0"/>
         <v>0.2666</v>
       </c>
       <c r="D5">
@@ -1491,7 +1703,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="5">
-        <f>0.1333*B6</f>
+        <f t="shared" si="0"/>
         <v>1.8662000000000001</v>
       </c>
       <c r="D6">
@@ -1507,7 +1719,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="5">
-        <f>0.1333*B7</f>
+        <f t="shared" si="0"/>
         <v>1.333</v>
       </c>
       <c r="D7">
@@ -1523,7 +1735,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="5">
-        <f>0.1333*B8</f>
+        <f t="shared" si="0"/>
         <v>0.93310000000000004</v>
       </c>
       <c r="D8">
@@ -1539,7 +1751,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="5">
-        <f>0.1333*B9</f>
+        <f t="shared" si="0"/>
         <v>0.79980000000000007</v>
       </c>
       <c r="D9">
@@ -1652,19 +1864,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="5" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -1678,7 +1893,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -1694,7 +1909,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -1710,9 +1925,837 @@
         <f>1000*C3*B3</f>
         <v>4352.4000000000005</v>
       </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <f>0.01*B6*D2</f>
+        <v>270</v>
+      </c>
+      <c r="D6" s="1">
+        <f>'Organ Mass'!C7</f>
+        <v>16050</v>
+      </c>
+      <c r="E6" s="7">
+        <f>C6/D6</f>
+        <v>1.6822429906542057E-2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="7">
+        <f>E6</f>
+        <v>1.6822429906542057E-2</v>
+      </c>
+      <c r="I6" s="7">
+        <f>E26</f>
+        <v>1.8715596330275232E-2</v>
+      </c>
+      <c r="J6" s="7">
+        <f>(H6+I6)/2</f>
+        <v>1.7769013118408644E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7">
+        <v>0.3</v>
+      </c>
+      <c r="C7" s="1">
+        <f>0.01*B7*D2</f>
+        <v>16.2</v>
+      </c>
+      <c r="D7" s="1">
+        <f>'Organ Mass'!C30</f>
+        <v>15</v>
+      </c>
+      <c r="E7" s="7">
+        <f>C7/D7</f>
+        <v>1.0799999999999998</v>
+      </c>
+      <c r="G7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H7" s="7">
+        <f>E7</f>
+        <v>1.0799999999999998</v>
+      </c>
+      <c r="I7" s="7">
+        <f>E27</f>
+        <v>1.08</v>
+      </c>
+      <c r="J7" s="7">
+        <f>(H7+I7)/2</f>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <f>0.01*B8*D2</f>
+        <v>270</v>
+      </c>
+      <c r="D8" s="1">
+        <f>'Organ Mass'!C5</f>
+        <v>10725</v>
+      </c>
+      <c r="E8" s="7">
+        <f>C8/D8</f>
+        <v>2.5174825174825177E-2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <f>E8</f>
+        <v>2.5174825174825177E-2</v>
+      </c>
+      <c r="I8" s="7">
+        <f>E28</f>
+        <v>2.5401691331923895E-2</v>
+      </c>
+      <c r="J8" s="7">
+        <f>(H8+I8)/2</f>
+        <v>2.5288258253374538E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1">
+        <f>0.01*B9*D2</f>
+        <v>648</v>
+      </c>
+      <c r="D9" s="1">
+        <f>'Organ Mass'!C6</f>
+        <v>1500</v>
+      </c>
+      <c r="E9" s="7">
+        <f>C9/D9</f>
+        <v>0.432</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <f>E9</f>
+        <v>0.432</v>
+      </c>
+      <c r="I9" s="7">
+        <f>E29</f>
+        <v>0.43589302325581408</v>
+      </c>
+      <c r="J9" s="7">
+        <f>(H9+I9)/2</f>
+        <v>0.43394651162790704</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <f>0.01*B10*D2</f>
+        <v>216</v>
+      </c>
+      <c r="D10" s="1">
+        <f>'Organ Mass'!C22</f>
+        <v>352.49999999999994</v>
+      </c>
+      <c r="E10" s="7">
+        <f>C10/D10</f>
+        <v>0.61276595744680862</v>
+      </c>
+      <c r="G10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="7">
+        <f>E10</f>
+        <v>0.61276595744680862</v>
+      </c>
+      <c r="I10" s="7">
+        <f>E30</f>
+        <v>0.76595744680851086</v>
+      </c>
+      <c r="J10" s="7">
+        <f>(H10+I10)/2</f>
+        <v>0.68936170212765968</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1">
+        <f>0.01*B11*D2</f>
+        <v>1026</v>
+      </c>
+      <c r="D11" s="1">
+        <f>'Organ Mass'!C9</f>
+        <v>330</v>
+      </c>
+      <c r="E11" s="7">
+        <f>C11/D11</f>
+        <v>3.1090909090909089</v>
+      </c>
+      <c r="G11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="7">
+        <f>E11</f>
+        <v>3.1090909090909089</v>
+      </c>
+      <c r="I11" s="7">
+        <f>E31</f>
+        <v>2.8068868921775909</v>
+      </c>
+      <c r="J11" s="7">
+        <f>(H11+I11)/2</f>
+        <v>2.9579889006342501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1">
+        <f>0.01*B12*D2</f>
+        <v>1350</v>
+      </c>
+      <c r="D12" s="1">
+        <f>'Organ Mass'!C11</f>
+        <v>1950</v>
+      </c>
+      <c r="E12" s="7">
+        <f>C12/D12</f>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="7">
+        <f>E12</f>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="I12" s="7">
+        <f>E32</f>
+        <v>0.75443023255813979</v>
+      </c>
+      <c r="J12" s="7">
+        <f>(H12+I12)/2</f>
+        <v>0.72336896243291604</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <f>0.01*B13*D2</f>
+        <v>324</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="G13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1">
+        <f>0.01*B14*D2</f>
+        <v>1026</v>
+      </c>
+      <c r="D14" s="1">
+        <f>'Organ Mass'!C8</f>
+        <v>1275</v>
+      </c>
+      <c r="E14" s="7">
+        <f>C14/D14</f>
+        <v>0.80470588235294116</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="7">
+        <f>E14</f>
+        <v>0.80470588235294116</v>
+      </c>
+      <c r="I14" s="7">
+        <f>E34</f>
+        <v>0.89742681258549972</v>
+      </c>
+      <c r="J14" s="7">
+        <f>(H14+I14)/2</f>
+        <v>0.85106634746922039</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15">
+        <v>2.5</v>
+      </c>
+      <c r="C15" s="1">
+        <f>0.01*B15*D2</f>
+        <v>135</v>
+      </c>
+      <c r="D15" s="1">
+        <f>'Organ Mass'!C34</f>
+        <v>570</v>
+      </c>
+      <c r="E15" s="7">
+        <f>C15/D15</f>
+        <v>0.23684210526315788</v>
+      </c>
+      <c r="G15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="7">
+        <f>E15</f>
+        <v>0.23684210526315788</v>
+      </c>
+      <c r="I15" s="7">
+        <f>E35</f>
+        <v>0.23684210526315791</v>
+      </c>
+      <c r="J15" s="7">
+        <f>(H15+I15)/2</f>
+        <v>0.23684210526315791</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1">
+        <f>0.01*B16*D2</f>
+        <v>918.00000000000011</v>
+      </c>
+      <c r="D16" s="1">
+        <f>'Organ Mass'!C26</f>
+        <v>30000</v>
+      </c>
+      <c r="E16" s="7">
+        <f>C16/D16</f>
+        <v>3.0600000000000002E-2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="7">
+        <f>E16</f>
+        <v>3.0600000000000002E-2</v>
+      </c>
+      <c r="I16" s="7">
+        <f>E36</f>
+        <v>2.1600000000000001E-2</v>
+      </c>
+      <c r="J16" s="7">
+        <f>(H16+I16)/2</f>
+        <v>2.6100000000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="1">
+        <f>'Organ Mass'!B27 * C16</f>
+        <v>110.16000000000001</v>
+      </c>
+      <c r="D17" s="1">
+        <f>'Organ Mass'!B27 * D16</f>
+        <v>3600</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="1">
+        <f>'Organ Mass'!B28 * C16</f>
+        <v>807.84000000000015</v>
+      </c>
+      <c r="D18" s="1">
+        <f>'Organ Mass'!B28 * D16</f>
+        <v>26400</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1">
+        <f>0.01*B19*D2</f>
+        <v>270</v>
+      </c>
+      <c r="D19" s="1">
+        <f>'Organ Mass'!C16</f>
+        <v>2775</v>
+      </c>
+      <c r="E19" s="7">
+        <f>C19/D19</f>
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="7">
+        <f>E19</f>
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="I19" s="7">
+        <f>E37</f>
+        <v>9.8174104336895066E-2</v>
+      </c>
+      <c r="J19" s="7">
+        <f>(H19+I19)/2</f>
+        <v>9.7735700817096177E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20">
+        <v>1.5</v>
+      </c>
+      <c r="C20" s="1">
+        <f>0.01*B20*D2</f>
+        <v>81</v>
+      </c>
+      <c r="D20" s="1">
+        <f>'Organ Mass'!C37</f>
+        <v>22.5</v>
+      </c>
+      <c r="E20" s="7">
+        <f>C20/D20</f>
+        <v>3.6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="7">
+        <f>E20</f>
+        <v>3.6</v>
+      </c>
+      <c r="I20" s="7">
+        <f>E38</f>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="J20" s="7">
+        <f>(H20+I20)/2</f>
+        <v>3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21">
+        <f>SUM(B6:B12,B15:B20)</f>
+        <v>96.3</v>
+      </c>
+      <c r="C21" s="1">
+        <f>SUM(C6:C12,C15:C16,C19:C20)</f>
+        <v>5200.2</v>
+      </c>
+      <c r="D21" s="1">
+        <f>SUM(D6:D12,D15:D16,D19:D20)</f>
+        <v>64290</v>
+      </c>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="1">
+        <f>SUM(C7:C12,C15,C19)</f>
+        <v>3931.2</v>
+      </c>
+      <c r="D23" s="1">
+        <f>SUM(D7:D12,D14:D16,D19:D20)</f>
+        <v>49515</v>
+      </c>
+      <c r="E23" s="7">
+        <f>C23/D23</f>
+        <v>7.9394122993032404E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26">
+        <v>8.5</v>
+      </c>
+      <c r="C26" s="1">
+        <f>0.01*B26*D3</f>
+        <v>369.95400000000006</v>
+      </c>
+      <c r="D26" s="1">
+        <f>Gender!D7</f>
+        <v>19767.150000000001</v>
+      </c>
+      <c r="E26" s="7">
+        <f>C26/D26</f>
+        <v>1.8715596330275232E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27">
+        <v>0.3</v>
+      </c>
+      <c r="C27" s="1">
+        <f>0.01*B27*D3</f>
+        <v>13.057200000000002</v>
+      </c>
+      <c r="D27" s="1">
+        <f>Gender!D30</f>
+        <v>12.090000000000002</v>
+      </c>
+      <c r="E27" s="7">
+        <f>C27/D27</f>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28" s="1">
+        <f>0.01*B28*D3</f>
+        <v>217.62000000000003</v>
+      </c>
+      <c r="D28" s="1">
+        <f>Gender!D5</f>
+        <v>8567.1460674157297</v>
+      </c>
+      <c r="E28" s="7">
+        <f>C28/D28</f>
+        <v>2.5401691331923895E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>12</v>
+      </c>
+      <c r="C29" s="1">
+        <f>0.01*B29*D3</f>
+        <v>522.28800000000001</v>
+      </c>
+      <c r="D29" s="1">
+        <f>Gender!D6</f>
+        <v>1198.2022471910109</v>
+      </c>
+      <c r="E29" s="7">
+        <f>C29/D29</f>
+        <v>0.43589302325581408</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1">
+        <f>0.01*B30*D3</f>
+        <v>217.62000000000003</v>
+      </c>
+      <c r="D30" s="1">
+        <f>Gender!C22</f>
+        <v>284.11499999999995</v>
+      </c>
+      <c r="E30" s="7">
+        <f>C30/D30</f>
+        <v>0.76595744680851086</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>17</v>
+      </c>
+      <c r="C31" s="1">
+        <f>0.01*B31*D3</f>
+        <v>739.90800000000013</v>
+      </c>
+      <c r="D31" s="1">
+        <f>Gender!D9</f>
+        <v>263.60449438202244</v>
+      </c>
+      <c r="E31" s="7">
+        <f>C31/D31</f>
+        <v>2.8068868921775909</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>27</v>
+      </c>
+      <c r="C32" s="1">
+        <f>0.01*B32*D3</f>
+        <v>1175.1480000000001</v>
+      </c>
+      <c r="D32" s="1">
+        <f>Gender!D11</f>
+        <v>1557.6629213483143</v>
+      </c>
+      <c r="E32" s="7">
+        <f>C32/D32</f>
+        <v>0.75443023255813979</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33" s="1">
+        <f>0.01*B33*D3</f>
+        <v>261.14400000000001</v>
+      </c>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34">
+        <v>21</v>
+      </c>
+      <c r="C34" s="1">
+        <f>0.01*B34*D3</f>
+        <v>914.00400000000013</v>
+      </c>
+      <c r="D34" s="1">
+        <f>Gender!D8</f>
+        <v>1018.4719101123592</v>
+      </c>
+      <c r="E34" s="7">
+        <f>C34/D34</f>
+        <v>0.89742681258549972</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35">
+        <v>2.5</v>
+      </c>
+      <c r="C35" s="1">
+        <f>0.01*B35*D3</f>
+        <v>108.81000000000002</v>
+      </c>
+      <c r="D35" s="1">
+        <f>Gender!D34</f>
+        <v>459.42</v>
+      </c>
+      <c r="E35" s="7">
+        <f>C35/D35</f>
+        <v>0.23684210526315791</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36">
+        <v>12</v>
+      </c>
+      <c r="C36" s="1">
+        <f>0.01*B36*D3</f>
+        <v>522.28800000000001</v>
+      </c>
+      <c r="D36" s="1">
+        <f>Gender!C26</f>
+        <v>24180</v>
+      </c>
+      <c r="E36" s="7">
+        <f>C36/D36</f>
+        <v>2.1600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1">
+        <f>0.01*B37*D3</f>
+        <v>217.62000000000003</v>
+      </c>
+      <c r="D37" s="1">
+        <f>Gender!D16</f>
+        <v>2216.6741573033705</v>
+      </c>
+      <c r="E37" s="7">
+        <f>C37/D37</f>
+        <v>9.8174104336895066E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38">
+        <v>1.5</v>
+      </c>
+      <c r="C38" s="1">
+        <f>0.01*B38*D3</f>
+        <v>65.286000000000001</v>
+      </c>
+      <c r="D38" s="1">
+        <f>Gender!D37</f>
+        <v>18.135000000000002</v>
+      </c>
+      <c r="E38" s="7">
+        <f>C38/D38</f>
+        <v>3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <f>SUM(B26:B32, B35:B38)</f>
+        <v>95.8</v>
+      </c>
+      <c r="C39" s="1">
+        <f>SUM(C26:C32,C35:C38)</f>
+        <v>4169.5992000000006</v>
+      </c>
+      <c r="D39" s="1">
+        <f>SUM(D26:D38)</f>
+        <v>59542.671797752817</v>
+      </c>
+      <c r="E39" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
HumModRepository - Adding scaling details to spreadsheet and normal values Web pages.
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6465" tabRatio="627" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6465" tabRatio="627" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Body Mass" sheetId="8" r:id="rId1"/>
@@ -14,30 +14,76 @@
     <sheet name="Pressure Gradients" sheetId="9" r:id="rId5"/>
     <sheet name="Organ Composition" sheetId="1" r:id="rId6"/>
     <sheet name="Organ Blood Flow" sheetId="7" r:id="rId7"/>
-    <sheet name="Calories" sheetId="2" r:id="rId8"/>
+    <sheet name="Systemic Blood Flow" sheetId="10" r:id="rId8"/>
     <sheet name="Vascular Conductance" sheetId="3" r:id="rId9"/>
+    <sheet name="Calories" sheetId="2" r:id="rId10"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
+    <definedName name="AdrenalMassFemale">'Organ Mass - Female'!$D$29</definedName>
+    <definedName name="AdrenalMassMale">'Organ Mass - Male'!$C$35</definedName>
     <definedName name="BaseMassFemale">'Organ Mass - Female'!$D$16</definedName>
     <definedName name="BaseMassMale">'Organ Mass - Male'!$C$16</definedName>
     <definedName name="BloodMass">'Organ Mass - Male'!$C$19</definedName>
     <definedName name="BodyMassFemale">'Body Mass'!$B$5</definedName>
     <definedName name="BodyMassMale">'Body Mass'!$B$4</definedName>
+    <definedName name="BoneFlowFemale">'Organ Blood Flow'!$H$11</definedName>
+    <definedName name="BoneFlowMale">'Organ Blood Flow'!$C$11</definedName>
+    <definedName name="BoneMassFemale">'Organ Mass - Female'!$D$4</definedName>
     <definedName name="BoneMassMale">'Organ Mass - Male'!$C$4</definedName>
+    <definedName name="BrainFlowFemale">'Organ Blood Flow'!$H$12</definedName>
+    <definedName name="BrainFlowMale">'Organ Blood Flow'!$C$12</definedName>
+    <definedName name="BrainMassFemale">'Organ Mass - Female'!$D$5</definedName>
     <definedName name="BrainMassMale">'Organ Mass - Male'!$C$5</definedName>
+    <definedName name="CardiacOutputFemale">'Organ Blood Flow'!$D$5</definedName>
+    <definedName name="CardiacOutputMale">'Organ Blood Flow'!$D$4</definedName>
     <definedName name="CoronaryGradient">'Pressure Gradients'!$D$6</definedName>
+    <definedName name="CoronarySinusOutflow">'Systemic Blood Flow'!$B$23</definedName>
+    <definedName name="FatFlowFemale">'Organ Blood Flow'!$H$9</definedName>
+    <definedName name="FatFlowMale">'Organ Blood Flow'!$C$9</definedName>
+    <definedName name="FatMassFemale">'Organ Mass - Female'!$D$6</definedName>
     <definedName name="FatMassMale">'Organ Mass - Male'!$C$6</definedName>
     <definedName name="FluidsMass">'Organ Mass - Male'!$C$23</definedName>
+    <definedName name="GIFlowFemale">'Organ Blood Flow'!$H$13</definedName>
+    <definedName name="GIFlowMale">'Organ Blood Flow'!$C$13</definedName>
+    <definedName name="GIMassFemale">'Organ Mass - Female'!$D$7</definedName>
     <definedName name="GIMassMale">'Organ Mass - Male'!$C$7</definedName>
     <definedName name="GITractGradient">'Pressure Gradients'!$D$5</definedName>
     <definedName name="GutH2OMass">'Organ Mass - Male'!$C$22</definedName>
+    <definedName name="HeartFlowFemale">'Organ Blood Flow'!$H$14</definedName>
+    <definedName name="HeartFlowMale">'Organ Blood Flow'!$C$14</definedName>
+    <definedName name="HeartMassFemale">'Organ Mass - Female'!$C$21</definedName>
+    <definedName name="HeartMassMale">'Organ Mass - Male'!$C$27</definedName>
     <definedName name="Hematocrit">'Organ Composition'!$B$19</definedName>
+    <definedName name="HepaticArtyFlowFemale">'Organ Blood Flow'!$H$15</definedName>
+    <definedName name="HepaticArtyFlowMale">'Organ Blood Flow'!$C$15</definedName>
     <definedName name="HepaticGradient">'Pressure Gradients'!$D$7</definedName>
+    <definedName name="HepaticVeinOutflow">'Systemic Blood Flow'!$B$19</definedName>
+    <definedName name="KidneyFlowFemale">'Organ Blood Flow'!$H$16</definedName>
+    <definedName name="KidneyFlowMale">'Organ Blood Flow'!$C$16</definedName>
+    <definedName name="KidneyMassFemale">'Organ Mass - Female'!$D$8</definedName>
     <definedName name="KidneyMassMale">'Organ Mass - Male'!$C$8</definedName>
     <definedName name="LeftAtrialPressure">'Blood Pressures'!$B$11</definedName>
+    <definedName name="LHeartFlowFemale">'Organ Blood Flow'!$H$27</definedName>
+    <definedName name="LHeartFlowMale">'Organ Blood Flow'!$C$27</definedName>
+    <definedName name="LHeartFractionFemale">'Organ Mass - Female'!$B$23</definedName>
+    <definedName name="LHeartFractionMale">'Organ Mass - Male'!$B$29</definedName>
+    <definedName name="LHeartMassFemale">'Organ Mass - Female'!$D$9</definedName>
     <definedName name="LHeartMassMale">'Organ Mass - Male'!$C$9</definedName>
+    <definedName name="LiverFlowFemale">'Organ Blood Flow'!$H$17</definedName>
+    <definedName name="LiverFlowMale">'Organ Blood Flow'!$C$17</definedName>
+    <definedName name="LiverMassFemale">'Organ Mass - Female'!$D$10</definedName>
     <definedName name="LiverMassMale">'Organ Mass - Male'!$C$10</definedName>
     <definedName name="LungH2OMass">'Organ Mass - Male'!$C$20</definedName>
+    <definedName name="LungMassFemale">'Organ Mass - Female'!$D$33</definedName>
+    <definedName name="LungMassMale">'Organ Mass - Male'!$C$39</definedName>
+    <definedName name="MuscleFlowFemale">'Organ Blood Flow'!$H$19</definedName>
+    <definedName name="MuscleFlowMale">'Organ Blood Flow'!$C$19</definedName>
+    <definedName name="MuscleMassFemale">'Organ Mass - Female'!$C$25</definedName>
+    <definedName name="MuscleMassMale">'Organ Mass - Male'!$C$31</definedName>
+    <definedName name="OtherFlowFemale">'Organ Blood Flow'!$H$33</definedName>
+    <definedName name="OtherFlowMale">'Organ Blood Flow'!$C$33</definedName>
+    <definedName name="OtherMassFemale">'Organ Mass - Female'!$D$11</definedName>
     <definedName name="OtherMassMale">'Organ Mass - Male'!$C$11</definedName>
     <definedName name="PeritoneumMass">'Organ Mass - Male'!$C$21</definedName>
     <definedName name="PulmArtyGradient">'Pressure Gradients'!$D$9</definedName>
@@ -46,23 +92,45 @@
     <definedName name="PulmCapysPressure">'Blood Pressures'!$B$9</definedName>
     <definedName name="PulmVeinsGradient">'Pressure Gradients'!$D$11</definedName>
     <definedName name="PulmVeinsPressure">'Blood Pressures'!$B$10</definedName>
+    <definedName name="RHeartFlowFemale">'Organ Blood Flow'!$H$26</definedName>
+    <definedName name="RHeartFlowMale">'Organ Blood Flow'!$C$26</definedName>
+    <definedName name="RHeartFractionFemale">'Organ Mass - Female'!$B$22</definedName>
+    <definedName name="RHeartFractionMale">'Organ Mass - Male'!$B$28</definedName>
+    <definedName name="RHeartMassFemale">'Organ Mass - Female'!$D$13</definedName>
     <definedName name="RHeartMassMale">'Organ Mass - Male'!$C$13</definedName>
     <definedName name="RightAtrialPressure">'Blood Pressures'!$B$7</definedName>
+    <definedName name="RMuscleFlowFemale">'Organ Blood Flow'!$H$30</definedName>
+    <definedName name="RMuscleFlowMale">'Organ Blood Flow'!$C$30</definedName>
+    <definedName name="RMuscleFractionFemale">'Organ Mass - Female'!$B$26</definedName>
+    <definedName name="RMuscleFractionMale">'Organ Mass - Male'!$B$32</definedName>
+    <definedName name="RMuscleMassFemale">'Organ Mass - Female'!$D$12</definedName>
     <definedName name="RMuscleMassMale">'Organ Mass - Male'!$C$12</definedName>
+    <definedName name="SkinFlowFemale">'Organ Blood Flow'!$H$20</definedName>
+    <definedName name="SkinFlowMale">'Organ Blood Flow'!$C$20</definedName>
+    <definedName name="SkinMassFemale">'Organ Mass - Female'!$D$15</definedName>
     <definedName name="SkinMassMale">'Organ Mass - Male'!$C$15</definedName>
+    <definedName name="SMuscleFlowFemale">'Organ Blood Flow'!$H$31</definedName>
+    <definedName name="SMuscleFlowMale">'Organ Blood Flow'!$C$31</definedName>
+    <definedName name="SMuscleFractionFemale">'Organ Mass - Female'!$B$27</definedName>
+    <definedName name="SMuscleFractionMale">'Organ Mass - Male'!$B$33</definedName>
+    <definedName name="SMuscleMassFemale">'Organ Mass - Female'!$D$14</definedName>
     <definedName name="SMuscleMassMale">'Organ Mass - Male'!$C$14</definedName>
     <definedName name="SplanchnicVeinsPressure">'Blood Pressures'!$B$6</definedName>
     <definedName name="SystemicArtysPressure">'Blood Pressures'!$B$4</definedName>
     <definedName name="SystemicGradient">'Pressure Gradients'!$D$4</definedName>
+    <definedName name="SystemicVeinOutflow">'Systemic Blood Flow'!$B$13</definedName>
     <definedName name="SystemicVeinsGradient">'Pressure Gradients'!$D$8</definedName>
     <definedName name="SystemicVeinsPressure">'Blood Pressures'!$B$5</definedName>
+    <definedName name="ThyroidMassFemale">'Organ Mass - Female'!$D$36</definedName>
+    <definedName name="ThyroidMassMale">'Organ Mass - Male'!$C$42</definedName>
+    <definedName name="VenousReturn">'Systemic Blood Flow'!$B$25</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="134">
   <si>
     <t>Bone</t>
   </si>
@@ -331,12 +399,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Cardiac Output</t>
-  </si>
-  <si>
-    <t>Organ - Male</t>
-  </si>
-  <si>
     <t>Adipose</t>
   </si>
   <si>
@@ -346,18 +408,6 @@
     <t>Lung</t>
   </si>
   <si>
-    <t>Organ - Female</t>
-  </si>
-  <si>
-    <t>% Cardiac Output</t>
-  </si>
-  <si>
-    <t>Blood Flow</t>
-  </si>
-  <si>
-    <t>Blood Flow (/G)</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
@@ -446,6 +496,42 @@
   </si>
   <si>
     <t>Ordinary</t>
+  </si>
+  <si>
+    <t>% CO</t>
+  </si>
+  <si>
+    <t>Flow</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>Flow (/G)</t>
+  </si>
+  <si>
+    <t>Systemic Blood Flow</t>
+  </si>
+  <si>
+    <t>Organ Blood Flow</t>
+  </si>
+  <si>
+    <t>OtherTissue</t>
+  </si>
+  <si>
+    <t>Systemic Vein Outflow</t>
+  </si>
+  <si>
+    <t>Hepatic Vein Outflow</t>
+  </si>
+  <si>
+    <t>Coronary Sinus Outflow</t>
+  </si>
+  <si>
+    <t>Venous Return</t>
+  </si>
+  <si>
+    <t>Pullmonary Veins Outflow</t>
   </si>
 </sst>
 </file>
@@ -487,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -498,6 +584,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,14 +892,14 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -854,6 +944,354 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>9700</v>
+      </c>
+      <c r="C2">
+        <v>90</v>
+      </c>
+      <c r="D2" s="3">
+        <f>C2/B2</f>
+        <v>9.2783505154639175E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1300</v>
+      </c>
+      <c r="C3">
+        <v>240</v>
+      </c>
+      <c r="D3" s="3">
+        <f>C3/B3</f>
+        <v>0.18461538461538463</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>16600</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3">
+        <f>C4/B4</f>
+        <v>1.8072289156626507E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1500</v>
+      </c>
+      <c r="C5">
+        <v>120</v>
+      </c>
+      <c r="D5" s="3">
+        <f>C5/B5</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>290</v>
+      </c>
+      <c r="C6">
+        <v>110</v>
+      </c>
+      <c r="D6" s="3">
+        <f>C6/B6</f>
+        <v>0.37931034482758619</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7" s="3">
+        <f>C7/B6</f>
+        <v>0.17241379310344829</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="D8" s="3">
+        <f>C8/B6</f>
+        <v>0.20689655172413793</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>260</v>
+      </c>
+      <c r="C9">
+        <v>130</v>
+      </c>
+      <c r="D9" s="3">
+        <f>C9/B9</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3">
+        <f>C10/B9</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>110</v>
+      </c>
+      <c r="D11" s="3">
+        <f>C11/B9</f>
+        <v>0.42307692307692307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>1750</v>
+      </c>
+      <c r="C12">
+        <v>190</v>
+      </c>
+      <c r="D12" s="3">
+        <f>C12/B12</f>
+        <v>0.10857142857142857</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>4100</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="D13" s="3">
+        <f>C13/B13</f>
+        <v>1.2195121951219513E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>3500</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14" s="3">
+        <f>C14/B14</f>
+        <v>8.5714285714285719E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3">
+        <f>C15/B14</f>
+        <v>2.8571428571428571E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16" s="3">
+        <f>C16/B14</f>
+        <v>5.7142857142857143E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+      <c r="D17" s="3">
+        <f>C17/B17</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3">
+        <f>C18/B17</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>22</v>
+      </c>
+      <c r="D19" s="3">
+        <f>C19/B17</f>
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>27000</v>
+      </c>
+      <c r="C20">
+        <v>140</v>
+      </c>
+      <c r="D20" s="3">
+        <f>C20/B20</f>
+        <v>5.185185185185185E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21">
+        <v>140</v>
+      </c>
+      <c r="D21" s="3">
+        <f>C21/B20</f>
+        <v>5.185185185185185E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>2550</v>
+      </c>
+      <c r="C22">
+        <v>40</v>
+      </c>
+      <c r="D22" s="3">
+        <f>C22/B22</f>
+        <v>1.5686274509803921E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23">
+        <f>SUM(B2:B22)</f>
+        <v>68600</v>
+      </c>
+      <c r="C23">
+        <f>SUM(C2:C6,C9,C12:C14,C17,C20,C22)</f>
+        <v>1195</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -861,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +1312,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -899,7 +1337,7 @@
         <v>14.3</v>
       </c>
       <c r="C4" s="1">
-        <f>10*B4*BodyMassMale</f>
+        <f t="shared" ref="C4:C15" si="0">10*B4*BodyMassMale</f>
         <v>10725</v>
       </c>
       <c r="D4" s="5">
@@ -915,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <f>10*B5*BodyMassMale</f>
+        <f t="shared" si="0"/>
         <v>1500</v>
       </c>
       <c r="D5" s="5">
@@ -931,7 +1369,7 @@
         <v>21.4</v>
       </c>
       <c r="C6" s="1">
-        <f>10*B6*BodyMassMale</f>
+        <f t="shared" si="0"/>
         <v>16050</v>
       </c>
       <c r="D6" s="5"/>
@@ -944,7 +1382,7 @@
         <v>1.7</v>
       </c>
       <c r="C7" s="1">
-        <f>10*B7*BodyMassMale</f>
+        <f t="shared" si="0"/>
         <v>1275</v>
       </c>
       <c r="D7" s="5">
@@ -960,7 +1398,7 @@
         <v>0.44</v>
       </c>
       <c r="C8" s="1">
-        <f>10*B8*BodyMassMale</f>
+        <f t="shared" si="0"/>
         <v>330</v>
       </c>
       <c r="D8" s="5">
@@ -977,7 +1415,7 @@
         <v>0.39009999999999995</v>
       </c>
       <c r="C9" s="1">
-        <f>10*B9*BodyMassMale</f>
+        <f t="shared" si="0"/>
         <v>292.57499999999993</v>
       </c>
       <c r="D9" s="5">
@@ -993,7 +1431,7 @@
         <v>2.6</v>
       </c>
       <c r="C10" s="1">
-        <f>10*B10*BodyMassMale</f>
+        <f t="shared" si="0"/>
         <v>1950</v>
       </c>
       <c r="D10" s="5">
@@ -1009,7 +1447,7 @@
         <v>4.7</v>
       </c>
       <c r="C11" s="1">
-        <f>10*B11*BodyMassMale</f>
+        <f t="shared" si="0"/>
         <v>3525</v>
       </c>
       <c r="D11" s="5">
@@ -1026,7 +1464,7 @@
         <v>4.8</v>
       </c>
       <c r="C12" s="1">
-        <f>10*B12*BodyMassMale</f>
+        <f t="shared" si="0"/>
         <v>3600</v>
       </c>
       <c r="D12" s="5">
@@ -1043,7 +1481,7 @@
         <v>7.9899999999999999E-2</v>
       </c>
       <c r="C13" s="1">
-        <f>10*B13*BodyMassMale</f>
+        <f t="shared" si="0"/>
         <v>59.924999999999997</v>
       </c>
       <c r="D13" s="5">
@@ -1060,7 +1498,7 @@
         <v>35.200000000000003</v>
       </c>
       <c r="C14" s="1">
-        <f>10*B14*BodyMassMale</f>
+        <f t="shared" si="0"/>
         <v>26400</v>
       </c>
       <c r="D14" s="5"/>
@@ -1073,7 +1511,7 @@
         <v>3.7</v>
       </c>
       <c r="C15" s="1">
-        <f>10*B15*BodyMassMale</f>
+        <f t="shared" si="0"/>
         <v>2775</v>
       </c>
       <c r="D15" s="5">
@@ -1083,7 +1521,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B16" s="5">
         <f>SUM(B4:B5,B7:B13,B15)</f>
@@ -1149,7 +1587,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B22" s="5">
         <v>1.3</v>
@@ -1161,7 +1599,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B23">
         <v>8.6999999999999993</v>
@@ -1176,7 +1614,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B25" s="5">
         <f>B17+B23</f>
@@ -1220,7 +1658,7 @@
         <v>51</v>
       </c>
       <c r="B29">
-        <f>1-B28</f>
+        <f>1-RHeartFractionMale</f>
         <v>0.83</v>
       </c>
       <c r="C29" s="1">
@@ -1257,7 +1695,7 @@
         <v>62</v>
       </c>
       <c r="B33">
-        <f>1-B32</f>
+        <f>1-RMuscleFractionMale</f>
         <v>0.88</v>
       </c>
       <c r="C33">
@@ -1276,7 +1714,7 @@
         <v>0.02</v>
       </c>
       <c r="C35" s="1">
-        <f>10*B35*BodyMassMale</f>
+        <f t="shared" ref="C35:C42" si="1">10*B35*BodyMassMale</f>
         <v>15</v>
       </c>
     </row>
@@ -1288,7 +1726,7 @@
         <v>0.21</v>
       </c>
       <c r="C36" s="1">
-        <f>10*B36*BodyMassMale</f>
+        <f t="shared" si="1"/>
         <v>157.5</v>
       </c>
     </row>
@@ -1300,7 +1738,7 @@
         <v>0.91</v>
       </c>
       <c r="C37" s="1">
-        <f>10*B37*BodyMassMale</f>
+        <f t="shared" si="1"/>
         <v>682.5</v>
       </c>
     </row>
@@ -1312,7 +1750,7 @@
         <v>0.53</v>
       </c>
       <c r="C38" s="1">
-        <f>10*B38*BodyMassMale</f>
+        <f t="shared" si="1"/>
         <v>397.50000000000006</v>
       </c>
     </row>
@@ -1324,7 +1762,7 @@
         <v>0.76</v>
       </c>
       <c r="C39" s="1">
-        <f>10*B39*BodyMassMale</f>
+        <f t="shared" si="1"/>
         <v>570</v>
       </c>
     </row>
@@ -1336,7 +1774,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="C40" s="1">
-        <f>10*B40*BodyMassMale</f>
+        <f t="shared" si="1"/>
         <v>105.00000000000001</v>
       </c>
     </row>
@@ -1348,7 +1786,7 @@
         <v>0.26</v>
       </c>
       <c r="C41" s="1">
-        <f>10*B41*BodyMassMale</f>
+        <f t="shared" si="1"/>
         <v>195</v>
       </c>
     </row>
@@ -1360,7 +1798,7 @@
         <v>0.03</v>
       </c>
       <c r="C42" s="1">
-        <f>10*B42*BodyMassMale</f>
+        <f t="shared" si="1"/>
         <v>22.5</v>
       </c>
     </row>
@@ -1374,8 +1812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,7 +1826,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1453,7 +1891,7 @@
         <v>4.897723998847594</v>
       </c>
       <c r="D7" s="1">
-        <f>0.01*C7*BaseMassFemale</f>
+        <f t="shared" ref="D7:D13" si="0">0.01*C7*BaseMassFemale</f>
         <v>1018.4719101123592</v>
       </c>
     </row>
@@ -1466,7 +1904,7 @@
         <v>1.2676462114664362</v>
       </c>
       <c r="D8" s="1">
-        <f>0.01*C8*BaseMassFemale</f>
+        <f t="shared" si="0"/>
         <v>263.60449438202244</v>
       </c>
     </row>
@@ -1479,7 +1917,7 @@
         <v>1.1238836070296743</v>
       </c>
       <c r="D9" s="1">
-        <f>0.01*C9*BaseMassFemale</f>
+        <f t="shared" si="0"/>
         <v>233.70934831460664</v>
       </c>
     </row>
@@ -1492,7 +1930,7 @@
         <v>7.4906367041198498</v>
       </c>
       <c r="D10" s="1">
-        <f>0.01*C10*BaseMassFemale</f>
+        <f t="shared" si="0"/>
         <v>1557.6629213483143</v>
       </c>
     </row>
@@ -1505,7 +1943,7 @@
         <v>13.540766349755113</v>
       </c>
       <c r="D11" s="1">
-        <f>0.01*C11*BaseMassFemale</f>
+        <f t="shared" si="0"/>
         <v>2815.7752808988762</v>
       </c>
     </row>
@@ -1531,7 +1969,7 @@
         <v>0.23019302794583693</v>
       </c>
       <c r="D13" s="1">
-        <f>0.01*C13*BaseMassFemale</f>
+        <f t="shared" si="0"/>
         <v>47.868179775280893</v>
       </c>
     </row>
@@ -1563,7 +2001,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C16" s="5">
         <f>SUM(C4:C5,C7:C13,C15)</f>
@@ -1611,12 +2049,13 @@
       <c r="A21" t="s">
         <v>49</v>
       </c>
-      <c r="B21">
-        <v>0.47</v>
+      <c r="B21" s="6">
+        <f>100*C21/D16</f>
+        <v>1.3540766349755113</v>
       </c>
       <c r="C21" s="1">
-        <f>10 * B21 *BodyMassFemale</f>
-        <v>284.11499999999995</v>
+        <f>D9+D13</f>
+        <v>281.57752808988755</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1625,11 +2064,12 @@
         <v>50</v>
       </c>
       <c r="B22">
-        <v>0.17</v>
+        <f>C22/C21</f>
+        <v>0.17000000000000004</v>
       </c>
       <c r="C22" s="1">
-        <f>B22 * C21</f>
-        <v>48.299549999999996</v>
+        <f>RHeartMassFemale</f>
+        <v>47.868179775280893</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1638,12 +2078,12 @@
         <v>51</v>
       </c>
       <c r="B23">
-        <f>1-B22</f>
+        <f>C23/C21</f>
         <v>0.83</v>
       </c>
       <c r="C23" s="1">
-        <f>B23 * C21</f>
-        <v>235.81544999999994</v>
+        <f>LHeartMassFemale</f>
+        <v>233.70934831460664</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -1655,12 +2095,13 @@
       <c r="A25" t="s">
         <v>60</v>
       </c>
-      <c r="B25">
-        <v>40</v>
+      <c r="B25" s="5">
+        <f>0.1*MuscleMassFemale/BodyMassFemale</f>
+        <v>28.957130509939503</v>
       </c>
       <c r="C25" s="1">
-        <f>10*B25*BodyMassFemale</f>
-        <v>24180</v>
+        <f>RMuscleMassFemale+SMuscleMassFemale</f>
+        <v>17504.585393258429</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1668,12 +2109,13 @@
       <c r="A26" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B26">
-        <v>0.12</v>
+      <c r="B26" s="6">
+        <f>RMuscleMassFemale/MuscleMassFemale</f>
+        <v>0.16428183408251101</v>
       </c>
       <c r="C26" s="1">
-        <f>C25*B26</f>
-        <v>2901.6</v>
+        <f>RMuscleMassFemale</f>
+        <v>2875.6853932584268</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -1681,13 +2123,13 @@
       <c r="A27" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B27">
-        <f>1-B26</f>
-        <v>0.88</v>
+      <c r="B27" s="6">
+        <f>SMuscleMassFemale/MuscleMassFemale</f>
+        <v>0.83571816591748893</v>
       </c>
       <c r="C27" s="1">
-        <f>C25*B27</f>
-        <v>21278.400000000001</v>
+        <f>SMuscleMassFemale</f>
+        <v>14628.900000000001</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -1699,7 +2141,7 @@
         <v>0.02</v>
       </c>
       <c r="D29" s="5">
-        <f>10*B29*BodyMassFemale</f>
+        <f t="shared" ref="D29:D36" si="1">10*B29*BodyMassFemale</f>
         <v>12.090000000000002</v>
       </c>
     </row>
@@ -1711,7 +2153,7 @@
         <v>0.21</v>
       </c>
       <c r="D30" s="5">
-        <f>10*B30*BodyMassFemale</f>
+        <f t="shared" si="1"/>
         <v>126.94500000000001</v>
       </c>
     </row>
@@ -1723,7 +2165,7 @@
         <v>0.91</v>
       </c>
       <c r="D31" s="5">
-        <f>10*B31*BodyMassFemale</f>
+        <f t="shared" si="1"/>
         <v>550.09500000000003</v>
       </c>
     </row>
@@ -1735,7 +2177,7 @@
         <v>0.53</v>
       </c>
       <c r="D32" s="5">
-        <f>10*B32*BodyMassFemale</f>
+        <f t="shared" si="1"/>
         <v>320.38500000000005</v>
       </c>
     </row>
@@ -1747,7 +2189,7 @@
         <v>0.76</v>
       </c>
       <c r="D33" s="5">
-        <f>10*B33*BodyMassFemale</f>
+        <f t="shared" si="1"/>
         <v>459.42</v>
       </c>
     </row>
@@ -1759,7 +2201,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="D34" s="5">
-        <f>10*B34*BodyMassFemale</f>
+        <f t="shared" si="1"/>
         <v>84.63000000000001</v>
       </c>
     </row>
@@ -1771,7 +2213,7 @@
         <v>0.26</v>
       </c>
       <c r="D35" s="5">
-        <f>10*B35*BodyMassFemale</f>
+        <f t="shared" si="1"/>
         <v>157.17000000000002</v>
       </c>
     </row>
@@ -1783,7 +2225,7 @@
         <v>0.03</v>
       </c>
       <c r="D36" s="5">
-        <f>10*B36*BodyMassFemale</f>
+        <f t="shared" si="1"/>
         <v>18.135000000000002</v>
       </c>
     </row>
@@ -1808,7 +2250,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2074,34 +2516,34 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B4">
         <f>SystemicArtysPressure</f>
@@ -2112,13 +2554,13 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <f>B4-C4</f>
+        <f t="shared" ref="D4:D11" si="0">B4-C4</f>
         <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B5">
         <f>SystemicArtysPressure</f>
@@ -2129,13 +2571,13 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <f>B5-C5</f>
+        <f t="shared" si="0"/>
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B6">
         <f>SystemicArtysPressure</f>
@@ -2146,13 +2588,13 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <f>B6-C6</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B7">
         <f>SplanchnicVeinsPressure</f>
@@ -2163,13 +2605,13 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <f>B7-C7</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B8">
         <f>SystemicVeinsPressure</f>
@@ -2180,13 +2622,13 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <f>B8-C8</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B9">
         <f>PulmArtyPressure</f>
@@ -2197,13 +2639,13 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <f>B9-C9</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B10">
         <f>PulmCapysPressure</f>
@@ -2214,13 +2656,13 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <f>B10-C10</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B11">
         <f>PulmVeinsPressure</f>
@@ -2231,7 +2673,7 @@
         <v>6</v>
       </c>
       <c r="D11">
-        <f>B11-C11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2263,30 +2705,30 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="I2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2315,7 +2757,7 @@
         <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2330,11 +2772,11 @@
         <v>0.32</v>
       </c>
       <c r="D4" s="1">
-        <f>B4*C4</f>
+        <f t="shared" ref="D4:D15" si="0">B4*C4</f>
         <v>3432</v>
       </c>
       <c r="E4" s="1">
-        <f>B4-D4</f>
+        <f t="shared" ref="E4:E15" si="1">B4-D4</f>
         <v>7293</v>
       </c>
       <c r="F4">
@@ -2364,11 +2806,11 @@
         <v>0.67</v>
       </c>
       <c r="D5" s="1">
-        <f>B5*C5</f>
+        <f t="shared" si="0"/>
         <v>1005.0000000000001</v>
       </c>
       <c r="E5" s="1">
-        <f>B5-D5</f>
+        <f t="shared" si="1"/>
         <v>494.99999999999989</v>
       </c>
       <c r="G5" s="1"/>
@@ -2385,11 +2827,11 @@
         <v>0.15</v>
       </c>
       <c r="D6" s="1">
-        <f>B6*C6</f>
+        <f t="shared" si="0"/>
         <v>2407.5</v>
       </c>
       <c r="E6" s="1">
-        <f>B6-D6</f>
+        <f t="shared" si="1"/>
         <v>13642.5</v>
       </c>
       <c r="F6">
@@ -2400,7 +2842,7 @@
         <v>12141.825000000001</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I6" s="1">
         <f>E6-G6</f>
@@ -2419,11 +2861,11 @@
         <v>0.67</v>
       </c>
       <c r="D7" s="1">
-        <f>B7*C7</f>
+        <f t="shared" si="0"/>
         <v>854.25</v>
       </c>
       <c r="E7" s="1">
-        <f>B7-D7</f>
+        <f t="shared" si="1"/>
         <v>420.75</v>
       </c>
       <c r="G7" s="1"/>
@@ -2440,11 +2882,11 @@
         <v>0.67</v>
       </c>
       <c r="D8" s="1">
-        <f>B8*C8</f>
+        <f t="shared" si="0"/>
         <v>221.10000000000002</v>
       </c>
       <c r="E8" s="1">
-        <f>B8-D8</f>
+        <f t="shared" si="1"/>
         <v>108.89999999999998</v>
       </c>
       <c r="G8" s="1"/>
@@ -2461,11 +2903,11 @@
         <v>0.67</v>
       </c>
       <c r="D9" s="1">
-        <f>B9*C9</f>
+        <f t="shared" si="0"/>
         <v>196.02524999999997</v>
       </c>
       <c r="E9" s="1">
-        <f>B9-D9</f>
+        <f t="shared" si="1"/>
         <v>96.54974999999996</v>
       </c>
       <c r="F9">
@@ -2495,11 +2937,11 @@
         <v>0.67</v>
       </c>
       <c r="D10" s="1">
-        <f>B10*C10</f>
+        <f t="shared" si="0"/>
         <v>1306.5</v>
       </c>
       <c r="E10" s="1">
-        <f>B10-D10</f>
+        <f t="shared" si="1"/>
         <v>643.5</v>
       </c>
       <c r="G10" s="1"/>
@@ -2516,11 +2958,11 @@
         <v>0.67</v>
       </c>
       <c r="D11" s="1">
-        <f>B11*C11</f>
+        <f t="shared" si="0"/>
         <v>2361.75</v>
       </c>
       <c r="E11" s="1">
-        <f>B11-D11</f>
+        <f t="shared" si="1"/>
         <v>1163.25</v>
       </c>
       <c r="G11" s="1"/>
@@ -2537,11 +2979,11 @@
         <v>0.79</v>
       </c>
       <c r="D12" s="1">
-        <f>B12*C12</f>
+        <f t="shared" si="0"/>
         <v>2844</v>
       </c>
       <c r="E12" s="1">
-        <f>B12-D12</f>
+        <f t="shared" si="1"/>
         <v>756</v>
       </c>
       <c r="F12">
@@ -2571,11 +3013,11 @@
         <v>0.67</v>
       </c>
       <c r="D13" s="1">
-        <f>B13*C13</f>
+        <f t="shared" si="0"/>
         <v>40.149749999999997</v>
       </c>
       <c r="E13" s="1">
-        <f>B13-D13</f>
+        <f t="shared" si="1"/>
         <v>19.77525</v>
       </c>
       <c r="F13">
@@ -2605,11 +3047,11 @@
         <v>0.79</v>
       </c>
       <c r="D14" s="1">
-        <f>B14*C14</f>
+        <f t="shared" si="0"/>
         <v>20856</v>
       </c>
       <c r="E14" s="1">
-        <f>B14-D14</f>
+        <f t="shared" si="1"/>
         <v>5544</v>
       </c>
       <c r="F14">
@@ -2639,11 +3081,11 @@
         <v>0.67</v>
       </c>
       <c r="D15" s="1">
-        <f>B15*C15</f>
+        <f t="shared" si="0"/>
         <v>1859.25</v>
       </c>
       <c r="E15" s="1">
-        <f>B15-D15</f>
+        <f t="shared" si="1"/>
         <v>915.75</v>
       </c>
     </row>
@@ -2675,7 +3117,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B19">
         <v>0.44</v>
@@ -2773,1230 +3215,1439 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="5" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>86</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4">
+        <f>BodyMassMale</f>
+        <v>75</v>
+      </c>
+      <c r="C4">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="D4">
+        <f>1000*C4*B4</f>
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="5">
+        <f>BodyMassFemale</f>
+        <v>60.45</v>
+      </c>
+      <c r="C5">
+        <f>C4</f>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <f>1000*C5*B5</f>
+        <v>4352.4000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" t="s">
+        <v>88</v>
+      </c>
+      <c r="L7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>125</v>
+      </c>
+      <c r="L8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <f>0.01*B9*D4</f>
+        <v>270</v>
+      </c>
+      <c r="D9" s="1">
+        <f>FatMassMale</f>
+        <v>16050</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" ref="E9:E17" si="0">C9/D9</f>
+        <v>1.6822429906542057E-2</v>
+      </c>
+      <c r="G9">
+        <v>8.5</v>
+      </c>
+      <c r="H9" s="1">
+        <f>0.01*G9*CardiacOutputFemale</f>
+        <v>369.95400000000006</v>
+      </c>
+      <c r="I9" s="1">
+        <f>FatMassFemale</f>
+        <v>19767.150000000001</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" ref="J9:J13" si="1">H9/I9</f>
+        <v>1.8715596330275232E-2</v>
+      </c>
+      <c r="L9" s="7">
+        <f>(E9+J9)/2</f>
+        <v>1.7769013118408644E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <v>0.3</v>
+      </c>
+      <c r="C10" s="1">
+        <f>0.01*B10*D4</f>
+        <v>16.2</v>
+      </c>
+      <c r="D10" s="1">
+        <f>AdrenalMassMale</f>
+        <v>15</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
+        <v>1.0799999999999998</v>
+      </c>
+      <c r="G10">
+        <v>0.3</v>
+      </c>
+      <c r="H10" s="1">
+        <f>0.01*G10*CardiacOutputFemale</f>
+        <v>13.057200000000002</v>
+      </c>
+      <c r="I10" s="1">
+        <f>AdrenalMassFemale</f>
+        <v>12.090000000000002</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>1.08</v>
+      </c>
+      <c r="L10" s="7">
+        <f>(E10+J10)/2</f>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <f>0.01*B11*D4</f>
+        <v>270</v>
+      </c>
+      <c r="D11" s="1">
+        <f>BoneMassMale</f>
+        <v>10725</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5174825174825177E-2</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1">
+        <f>0.01*G11*CardiacOutputFemale</f>
+        <v>217.62000000000003</v>
+      </c>
+      <c r="I11" s="1">
+        <f>BoneMassFemale</f>
+        <v>8567.1460674157297</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="1"/>
+        <v>2.5401691331923895E-2</v>
+      </c>
+      <c r="L11" s="7">
+        <f>(E11+J11)/2</f>
+        <v>2.5288258253374538E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1">
+        <f>0.01*B12*D4</f>
+        <v>648</v>
+      </c>
+      <c r="D12" s="1">
+        <f>BrainMassMale</f>
+        <v>1500</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.432</v>
+      </c>
+      <c r="G12">
+        <v>12</v>
+      </c>
+      <c r="H12" s="1">
+        <f>0.01*G12*CardiacOutputFemale</f>
+        <v>522.28800000000001</v>
+      </c>
+      <c r="I12" s="1">
+        <f>BrainMassFemale</f>
+        <v>1198.2022471910109</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="1"/>
+        <v>0.43589302325581408</v>
+      </c>
+      <c r="L12" s="7">
+        <f>(E12+J12)/2</f>
+        <v>0.43394651162790704</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" t="e">
-        <f>'Organ Mass - Male'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C2">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="D2" t="e">
-        <f>1000*C2*B2</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="5" t="e">
-        <f>'Organ Mass - Female'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C3">
-        <f>C2</f>
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="D3" s="1" t="e">
-        <f>1000*C3*B3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" t="s">
-        <v>87</v>
-      </c>
-      <c r="I5" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C13" s="1">
+        <f>0.01*B13*CardiacOutputMale</f>
+        <v>1026</v>
+      </c>
+      <c r="D13" s="1">
+        <f>GIMassMale</f>
+        <v>1275</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.80470588235294116</v>
+      </c>
+      <c r="G13">
+        <v>21</v>
+      </c>
+      <c r="H13" s="1">
+        <f>0.01*G13*CardiacOutputFemale</f>
+        <v>914.00400000000013</v>
+      </c>
+      <c r="I13" s="1">
+        <f>GIMassFemale</f>
+        <v>1018.4719101123592</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="1"/>
+        <v>0.89742681258549972</v>
+      </c>
+      <c r="L13" s="7">
+        <f>(E13+J13)/2</f>
+        <v>0.85106634746922039</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1">
+        <f>0.01*B14*CardiacOutputMale</f>
+        <v>216</v>
+      </c>
+      <c r="D14" s="1">
+        <f>HeartMassMale</f>
+        <v>352.49999999999994</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.61276595744680862</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1">
+        <f>0.01*G14*CardiacOutputFemale</f>
+        <v>217.62000000000003</v>
+      </c>
+      <c r="I14" s="1">
+        <f>HeartMassFemale</f>
+        <v>281.57752808988755</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" ref="J14" si="2">H14/I14</f>
+        <v>0.77285997031172726</v>
+      </c>
+      <c r="L14" s="7">
+        <f>(E14+J14)/2</f>
+        <v>0.69281296387926794</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1">
+        <f>0.01*B15*CardiacOutputMale</f>
+        <v>324</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="7"/>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15" s="1">
+        <f>0.01*G15*CardiacOutputFemale</f>
+        <v>261.14400000000001</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="7"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1">
+        <f>0.01*B16*D4</f>
+        <v>1026</v>
+      </c>
+      <c r="D16" s="1">
+        <f>KidneyMassMale</f>
+        <v>330</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="0"/>
+        <v>3.1090909090909089</v>
+      </c>
+      <c r="G16">
+        <v>17</v>
+      </c>
+      <c r="H16" s="1">
+        <f>0.01*G16*CardiacOutputFemale</f>
+        <v>739.90800000000013</v>
+      </c>
+      <c r="I16" s="1">
+        <f>KidneyMassFemale</f>
+        <v>263.60449438202244</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" ref="J16:J17" si="3">H16/I16</f>
+        <v>2.8068868921775909</v>
+      </c>
+      <c r="L16" s="7">
+        <f>(E16+J16)/2</f>
+        <v>2.9579889006342501</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1">
+        <f>0.01*B17*D4</f>
+        <v>1350</v>
+      </c>
+      <c r="D17" s="1">
+        <f>LiverMassMale</f>
+        <v>1950</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="G17">
+        <v>27</v>
+      </c>
+      <c r="H17" s="1">
+        <f>0.01*G17*CardiacOutputFemale</f>
+        <v>1175.1480000000001</v>
+      </c>
+      <c r="I17" s="1">
+        <f>LiverMassFemale</f>
+        <v>1557.6629213483143</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="3"/>
+        <v>0.75443023255813979</v>
+      </c>
+      <c r="L17" s="7">
+        <f>(E17+J17)/2</f>
+        <v>0.72336896243291604</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>91</v>
       </c>
-      <c r="B6">
+      <c r="B18">
+        <v>2.5</v>
+      </c>
+      <c r="C18" s="1">
+        <f>0.01*B18*D4</f>
+        <v>135</v>
+      </c>
+      <c r="D18" s="1">
+        <f>LungMassMale</f>
+        <v>570</v>
+      </c>
+      <c r="E18" s="7">
+        <f>C18/D18</f>
+        <v>0.23684210526315788</v>
+      </c>
+      <c r="G18">
+        <v>2.5</v>
+      </c>
+      <c r="H18" s="1">
+        <f>0.01*G18*CardiacOutputFemale</f>
+        <v>108.81000000000002</v>
+      </c>
+      <c r="I18" s="1">
+        <f>LungMassFemale</f>
+        <v>459.42</v>
+      </c>
+      <c r="J18" s="7">
+        <f>H18/I18</f>
+        <v>0.23684210526315791</v>
+      </c>
+      <c r="L18" s="7">
+        <f>(E18+J18)/2</f>
+        <v>0.23684210526315791</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1">
+        <f>0.01*B19*D4</f>
+        <v>918.00000000000011</v>
+      </c>
+      <c r="D19" s="1">
+        <f>MuscleMassMale</f>
+        <v>30000</v>
+      </c>
+      <c r="E19" s="7">
+        <f>C19/D19</f>
+        <v>3.0600000000000002E-2</v>
+      </c>
+      <c r="G19">
+        <v>12</v>
+      </c>
+      <c r="H19" s="1">
+        <f>0.01*G19*CardiacOutputFemale</f>
+        <v>522.28800000000001</v>
+      </c>
+      <c r="I19" s="1">
+        <f>MuscleMassFemale</f>
+        <v>17504.585393258429</v>
+      </c>
+      <c r="J19" s="7">
+        <f>H19/I19</f>
+        <v>2.9837210551764894E-2</v>
+      </c>
+      <c r="L19" s="7">
+        <f>(E19+J19)/2</f>
+        <v>3.0218605275882448E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="e">
-        <f>0.01*B6*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D6" s="1">
-        <f>'Organ Mass - Male'!C6</f>
-        <v>16050</v>
-      </c>
-      <c r="E6" s="7" t="e">
-        <f t="shared" ref="E6:E12" si="0">C6/D6</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H6" s="7" t="e">
-        <f t="shared" ref="H6:H12" si="1">E6</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I6" s="7" t="e">
-        <f t="shared" ref="I6:I12" si="2">E26</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J6" s="7" t="e">
-        <f t="shared" ref="J6:J12" si="3">(H6+I6)/2</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B7">
-        <v>0.3</v>
-      </c>
-      <c r="C7" s="1" t="e">
-        <f>0.01*B7*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D7" s="1">
-        <f>'Organ Mass - Male'!C35</f>
-        <v>15</v>
-      </c>
-      <c r="E7" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="G7" t="s">
-        <v>92</v>
-      </c>
-      <c r="H7" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I7" s="7" t="e">
-        <f t="shared" si="2"/>
-        <v>#REF!</v>
-      </c>
-      <c r="J7" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8">
+      <c r="C20" s="1">
+        <f>0.01*B20*D4</f>
+        <v>270</v>
+      </c>
+      <c r="D20" s="1">
+        <f>SkinMassMale</f>
+        <v>2775</v>
+      </c>
+      <c r="E20" s="7">
+        <f>C20/D20</f>
+        <v>9.7297297297297303E-2</v>
+      </c>
+      <c r="G20">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="e">
-        <f>0.01*B8*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D8" s="1">
-        <f>'Organ Mass - Male'!C4</f>
-        <v>10725</v>
-      </c>
-      <c r="E8" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="G8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I8" s="7" t="e">
-        <f t="shared" si="2"/>
-        <v>#REF!</v>
-      </c>
-      <c r="J8" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="e">
-        <f>0.01*B9*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D9" s="1">
-        <f>'Organ Mass - Male'!C5</f>
-        <v>1500</v>
-      </c>
-      <c r="E9" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="G9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I9" s="7" t="e">
-        <f t="shared" si="2"/>
-        <v>#REF!</v>
-      </c>
-      <c r="J9" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1" t="e">
-        <f>0.01*B10*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D10" s="1">
-        <f>'Organ Mass - Male'!C27</f>
-        <v>352.49999999999994</v>
-      </c>
-      <c r="E10" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="G10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I10" s="7" t="e">
-        <f t="shared" si="2"/>
-        <v>#REF!</v>
-      </c>
-      <c r="J10" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>19</v>
-      </c>
-      <c r="C11" s="1" t="e">
-        <f>0.01*B11*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D11" s="1">
-        <f>'Organ Mass - Male'!C8</f>
-        <v>330</v>
-      </c>
-      <c r="E11" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="G11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I11" s="7" t="e">
-        <f t="shared" si="2"/>
-        <v>#REF!</v>
-      </c>
-      <c r="J11" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="e">
-        <f>0.01*B12*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D12" s="1">
-        <f>'Organ Mass - Male'!C10</f>
-        <v>1950</v>
-      </c>
-      <c r="E12" s="7" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="G12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="7" t="e">
-        <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I12" s="7" t="e">
-        <f t="shared" si="2"/>
-        <v>#REF!</v>
-      </c>
-      <c r="J12" s="7" t="e">
-        <f t="shared" si="3"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13">
-        <v>6</v>
-      </c>
-      <c r="C13" s="1" t="e">
-        <f>0.01*B13*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="G13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="e">
-        <f>0.01*B14*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D14" s="1">
-        <f>'Organ Mass - Male'!C7</f>
-        <v>1275</v>
-      </c>
-      <c r="E14" s="7" t="e">
-        <f>C14/D14</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="7" t="e">
-        <f>E14</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I14" s="7" t="e">
-        <f>E34</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J14" s="7" t="e">
-        <f>(H14+I14)/2</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15">
-        <v>2.5</v>
-      </c>
-      <c r="C15" s="1" t="e">
-        <f>0.01*B15*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D15" s="1">
-        <f>'Organ Mass - Male'!C39</f>
-        <v>570</v>
-      </c>
-      <c r="E15" s="7" t="e">
-        <f>C15/D15</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G15" t="s">
-        <v>93</v>
-      </c>
-      <c r="H15" s="7" t="e">
-        <f>E15</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I15" s="7" t="e">
-        <f>E35</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J15" s="7" t="e">
-        <f>(H15+I15)/2</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="e">
-        <f>0.01*B16*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D16" s="1">
-        <f>'Organ Mass - Male'!C31</f>
-        <v>30000</v>
-      </c>
-      <c r="E16" s="7" t="e">
-        <f>C16/D16</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" s="7" t="e">
-        <f>E16</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I16" s="7" t="e">
-        <f>E36</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J16" s="7" t="e">
-        <f>(H16+I16)/2</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="1" t="e">
-        <f>'Organ Mass - Male'!B32 * C16</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D17" s="1">
-        <f>'Organ Mass - Male'!B32 * D16</f>
-        <v>3600</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="1" t="e">
-        <f>'Organ Mass - Male'!B33 * C16</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D18" s="1">
-        <f>'Organ Mass - Male'!B33 * D16</f>
-        <v>26400</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19">
-        <v>5</v>
-      </c>
-      <c r="C19" s="1" t="e">
-        <f>0.01*B19*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D19" s="1">
-        <f>'Organ Mass - Male'!C15</f>
-        <v>2775</v>
-      </c>
-      <c r="E19" s="7" t="e">
-        <f>C19/D19</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="7" t="e">
-        <f>E19</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I19" s="7" t="e">
-        <f>E37</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J19" s="7" t="e">
-        <f>(H19+I19)/2</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="H20" s="1">
+        <f>0.01*G20*CardiacOutputFemale</f>
+        <v>217.62000000000003</v>
+      </c>
+      <c r="I20" s="1">
+        <f>SkinMassFemale</f>
+        <v>2216.6741573033705</v>
+      </c>
+      <c r="J20" s="7">
+        <f>H20/I20</f>
+        <v>9.8174104336895066E-2</v>
+      </c>
+      <c r="L20" s="7">
+        <f>(E20+J20)/2</f>
+        <v>9.7735700817096177E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>59</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>1.5</v>
       </c>
-      <c r="C20" s="1" t="e">
-        <f>0.01*B20*D2</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D20" s="1">
-        <f>'Organ Mass - Male'!C42</f>
+      <c r="C21" s="1">
+        <f>0.01*B21*D4</f>
+        <v>81</v>
+      </c>
+      <c r="D21" s="1">
+        <f>ThyroidMassMale</f>
         <v>22.5</v>
       </c>
-      <c r="E20" s="7" t="e">
-        <f>C20/D20</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G20" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="7" t="e">
-        <f>E20</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I20" s="7" t="e">
-        <f>E38</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J20" s="7" t="e">
-        <f>(H20+I20)/2</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21">
-        <f>SUM(B6:B12,B15:B20)</f>
-        <v>96.3</v>
-      </c>
-      <c r="C21" s="1" t="e">
-        <f>SUM(C6:C12,C15:C16,C19:C20)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D21" s="1">
-        <f>SUM(D6:D12,D15:D16,D19:D20)</f>
-        <v>64290</v>
-      </c>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E21" s="7">
+        <f>C21/D21</f>
+        <v>3.6</v>
+      </c>
+      <c r="G21">
+        <v>1.5</v>
+      </c>
+      <c r="H21" s="1">
+        <f>0.01*G21*CardiacOutputFemale</f>
+        <v>65.286000000000001</v>
+      </c>
+      <c r="I21" s="1">
+        <f>ThyroidMassFemale</f>
+        <v>18.135000000000002</v>
+      </c>
+      <c r="J21" s="7">
+        <f>H21/I21</f>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="L21" s="7">
+        <f>(E21+J21)/2</f>
+        <v>3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="7"/>
+      <c r="L22" s="7"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="1" t="e">
-        <f>SUM(C7:C12,C15,C19)</f>
-        <v>#REF!</v>
+      <c r="C23" s="1">
+        <f>SUM(C10:C12,C14,C16:C18,C20:C21)</f>
+        <v>4012.2</v>
       </c>
       <c r="D23" s="1">
-        <f>SUM(D7:D12,D14:D16,D19:D20)</f>
+        <f>SUM(D10:D17,D18:D19,D20:D21)</f>
         <v>49515</v>
       </c>
-      <c r="E23" s="7" t="e">
+      <c r="E23" s="7">
         <f>C23/D23</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.1029990911844887E-2</v>
+      </c>
+      <c r="H23" s="1">
+        <f>SUM(H10:H12,H14,H16:H18,H20:H21)</f>
+        <v>3277.3572000000004</v>
+      </c>
+      <c r="I23" s="1">
+        <f>SUM(I10:I17,I18:I19,I20:I21)</f>
+        <v>33097.569719101128</v>
+      </c>
+      <c r="J23" s="7">
+        <f>H23/I23</f>
+        <v>9.9021083052771269E-2</v>
+      </c>
+      <c r="L23" s="7">
+        <f>(E23+J23)/2</f>
+        <v>9.0025536982308085E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="C25" s="1">
+        <f>HeartFlowMale</f>
+        <v>216</v>
+      </c>
+      <c r="D25" s="1">
+        <f>HeartMassMale</f>
+        <v>352.49999999999994</v>
+      </c>
       <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>91</v>
+      <c r="H25" s="1">
+        <f>HeartFlowFemale</f>
+        <v>217.62000000000003</v>
+      </c>
+      <c r="I25" s="1">
+        <f>HeartMassFemale</f>
+        <v>281.57752808988755</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B26">
-        <v>8.5</v>
-      </c>
-      <c r="C26" s="1" t="e">
-        <f>0.01*B26*D3</f>
-        <v>#REF!</v>
+        <f>RHeartFractionMale</f>
+        <v>0.17</v>
+      </c>
+      <c r="C26" s="1">
+        <f>RHeartFractionMale*HeartFlowMale</f>
+        <v>36.720000000000006</v>
       </c>
       <c r="D26" s="1">
-        <f>'Organ Mass - Female'!D6</f>
-        <v>19767.150000000001</v>
-      </c>
-      <c r="E26" s="7" t="e">
-        <f t="shared" ref="E26:E32" si="4">C26/D26</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>92</v>
+        <f>RHeartMassMale</f>
+        <v>59.924999999999997</v>
+      </c>
+      <c r="E26" s="7">
+        <f>RHeartFlowMale/RHeartMassMale</f>
+        <v>0.61276595744680862</v>
+      </c>
+      <c r="G26">
+        <f>RHeartFractionFemale</f>
+        <v>0.17000000000000004</v>
+      </c>
+      <c r="H26" s="1">
+        <f>RHeartFractionFemale*HeartFlowFemale</f>
+        <v>36.995400000000018</v>
+      </c>
+      <c r="I26" s="1">
+        <f>RHeartMassFemale</f>
+        <v>47.868179775280893</v>
+      </c>
+      <c r="J26" s="7">
+        <f>RHeartFlowFemale/RHeartMassFemale</f>
+        <v>0.77285997031172737</v>
+      </c>
+      <c r="L26" s="7">
+        <f>(E26+J26)/2</f>
+        <v>0.69281296387926794</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B27">
-        <v>0.3</v>
-      </c>
-      <c r="C27" s="1" t="e">
-        <f>0.01*B27*D3</f>
-        <v>#REF!</v>
+        <f>LHeartFractionMale</f>
+        <v>0.83</v>
+      </c>
+      <c r="C27" s="1">
+        <f>LHeartFractionMale*HeartFlowMale</f>
+        <v>179.28</v>
       </c>
       <c r="D27" s="1">
-        <f>'Organ Mass - Female'!D29</f>
-        <v>12.090000000000002</v>
-      </c>
-      <c r="E27" s="7" t="e">
-        <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28">
-        <v>5</v>
-      </c>
-      <c r="C28" s="1" t="e">
-        <f>0.01*B28*D3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D28" s="1">
-        <f>'Organ Mass - Female'!D4</f>
-        <v>8567.1460674157297</v>
-      </c>
-      <c r="E28" s="7" t="e">
-        <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <f>LHeartMassMale</f>
+        <v>292.57499999999993</v>
+      </c>
+      <c r="E27" s="7">
+        <f>LHeartFlowMale/LHeartMassMale</f>
+        <v>0.61276595744680862</v>
+      </c>
+      <c r="G27">
+        <f>LHeartFractionFemale</f>
+        <v>0.83</v>
+      </c>
+      <c r="H27" s="1">
+        <f>LHeartFractionFemale*HeartFlowFemale</f>
+        <v>180.62460000000002</v>
+      </c>
+      <c r="I27" s="1">
+        <f>LHeartMassFemale</f>
+        <v>233.70934831460664</v>
+      </c>
+      <c r="J27" s="7">
+        <f>LHeartFlowFemale/LHeartMassFemale</f>
+        <v>0.77285997031172726</v>
+      </c>
+      <c r="L27" s="7">
+        <f>(E27+J27)/2</f>
+        <v>0.69281296387926794</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="7"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29">
-        <v>12</v>
-      </c>
-      <c r="C29" s="1" t="e">
-        <f>0.01*B29*D3</f>
-        <v>#REF!</v>
+        <v>60</v>
+      </c>
+      <c r="C29" s="1">
+        <f>MuscleFlowMale</f>
+        <v>918.00000000000011</v>
       </c>
       <c r="D29" s="1">
-        <f>'Organ Mass - Female'!D5</f>
-        <v>1198.2022471910109</v>
-      </c>
-      <c r="E29" s="7" t="e">
-        <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>49</v>
+        <f>MuscleMassMale</f>
+        <v>30000</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="H29" s="1">
+        <f>MuscleFlowFemale</f>
+        <v>522.28800000000001</v>
+      </c>
+      <c r="I29" s="1">
+        <f>MuscleMassFemale</f>
+        <v>17504.585393258429</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="B30">
-        <v>5</v>
-      </c>
-      <c r="C30" s="1" t="e">
-        <f>0.01*B30*D3</f>
-        <v>#REF!</v>
+        <f>RMuscleFractionMale</f>
+        <v>0.12</v>
+      </c>
+      <c r="C30" s="1">
+        <f>RMuscleFractionMale*MuscleFlowMale</f>
+        <v>110.16000000000001</v>
       </c>
       <c r="D30" s="1">
-        <f>'Organ Mass - Female'!C21</f>
-        <v>284.11499999999995</v>
-      </c>
-      <c r="E30" s="7" t="e">
-        <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>4</v>
+        <f>RMuscleMassMale</f>
+        <v>3600</v>
+      </c>
+      <c r="E30" s="7">
+        <f>RMuscleFlowMale/RMuscleMassMale</f>
+        <v>3.0600000000000002E-2</v>
+      </c>
+      <c r="G30" s="6">
+        <f>RMuscleFractionFemale</f>
+        <v>0.16428183408251101</v>
+      </c>
+      <c r="H30" s="1">
+        <f>RMuscleFractionFemale*MuscleFlowFemale</f>
+        <v>85.80243055928652</v>
+      </c>
+      <c r="I30" s="1">
+        <f>RMuscleMassFemale</f>
+        <v>2875.6853932584268</v>
+      </c>
+      <c r="J30" s="7">
+        <f>RMuscleFlowFemale/RMuscleMassFemale</f>
+        <v>2.9837210551764897E-2</v>
+      </c>
+      <c r="L30" s="7">
+        <f>(E30+J30)/2</f>
+        <v>3.0218605275882451E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="B31">
-        <v>17</v>
-      </c>
-      <c r="C31" s="1" t="e">
-        <f>0.01*B31*D3</f>
-        <v>#REF!</v>
+        <f>SMuscleFractionMale</f>
+        <v>0.88</v>
+      </c>
+      <c r="C31" s="1">
+        <f>SMuscleFractionMale*MuscleFlowMale</f>
+        <v>807.84000000000015</v>
       </c>
       <c r="D31" s="1">
-        <f>'Organ Mass - Female'!D8</f>
-        <v>263.60449438202244</v>
-      </c>
-      <c r="E31" s="7" t="e">
-        <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32">
-        <v>27</v>
-      </c>
-      <c r="C32" s="1" t="e">
-        <f>0.01*B32*D3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D32" s="1">
-        <f>'Organ Mass - Female'!D10</f>
-        <v>1557.6629213483143</v>
-      </c>
-      <c r="E32" s="7" t="e">
-        <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33">
-        <v>6</v>
-      </c>
-      <c r="C33" s="1" t="e">
-        <f>0.01*B33*D3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34">
-        <v>21</v>
-      </c>
-      <c r="C34" s="1" t="e">
-        <f>0.01*B34*D3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D34" s="1">
-        <f>'Organ Mass - Female'!D7</f>
-        <v>1018.4719101123592</v>
-      </c>
-      <c r="E34" s="7" t="e">
-        <f>C34/D34</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35">
-        <v>2.5</v>
-      </c>
-      <c r="C35" s="1" t="e">
-        <f>0.01*B35*D3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D35" s="1">
-        <f>'Organ Mass - Female'!D33</f>
-        <v>459.42</v>
-      </c>
-      <c r="E35" s="7" t="e">
-        <f>C35/D35</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36">
-        <v>12</v>
-      </c>
-      <c r="C36" s="1" t="e">
-        <f>0.01*B36*D3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D36" s="1">
-        <f>'Organ Mass - Female'!C25</f>
-        <v>24180</v>
-      </c>
-      <c r="E36" s="7" t="e">
-        <f>C36/D36</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="C37" s="1" t="e">
-        <f>0.01*B37*D3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D37" s="1">
-        <f>'Organ Mass - Female'!D15</f>
-        <v>2216.6741573033705</v>
-      </c>
-      <c r="E37" s="7" t="e">
-        <f>C37/D37</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38">
-        <v>1.5</v>
-      </c>
-      <c r="C38" s="1" t="e">
-        <f>0.01*B38*D3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D38" s="1">
-        <f>'Organ Mass - Female'!D36</f>
-        <v>18.135000000000002</v>
-      </c>
-      <c r="E38" s="7" t="e">
-        <f>C38/D38</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39">
-        <f>SUM(B26:B32, B35:B38)</f>
-        <v>95.8</v>
-      </c>
-      <c r="C39" s="1" t="e">
-        <f>SUM(C26:C32,C35:C38)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D39" s="1">
-        <f>SUM(D26:D38)</f>
-        <v>59542.671797752817</v>
-      </c>
+        <f>SMuscleMassMale</f>
+        <v>26400</v>
+      </c>
+      <c r="E31" s="7">
+        <f>SMuscleFlowMale/SMuscleMassMale</f>
+        <v>3.0600000000000006E-2</v>
+      </c>
+      <c r="G31" s="6">
+        <f>SMuscleFractionFemale</f>
+        <v>0.83571816591748893</v>
+      </c>
+      <c r="H31" s="1">
+        <f>SMuscleFractionFemale*MuscleFlowFemale</f>
+        <v>436.48556944071345</v>
+      </c>
+      <c r="I31" s="1">
+        <f>SMuscleMassFemale</f>
+        <v>14628.900000000001</v>
+      </c>
+      <c r="J31" s="7">
+        <f>SMuscleFlowFemale/SMuscleMassFemale</f>
+        <v>2.983721055176489E-2</v>
+      </c>
+      <c r="L31" s="7">
+        <f>(E31+J31)/2</f>
+        <v>3.0218605275882448E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="9">
+        <f>CardiacOutputMale-FatFlowMale-BoneFlowMale-BrainFlowMale-HeartFlowMale-KidneyFlowMale-LiverFlowMale-MuscleFlowMale-SkinFlowMale</f>
+        <v>431.99999999999989</v>
+      </c>
+      <c r="D33">
+        <v>3525</v>
+      </c>
+      <c r="E33" s="7">
+        <f>C33/D33</f>
+        <v>0.12255319148936167</v>
+      </c>
+      <c r="H33" s="1">
+        <f>CardiacOutputFemale-FatFlowFemale-BoneFlowFemale-BrainFlowFemale-HeartFlowFemale-KidneyFlowFemale-LiverFlowFemale-MuscleFlowFemale-SkinFlowFemale</f>
+        <v>369.95400000000006</v>
+      </c>
+      <c r="I33" s="1">
+        <f>D33*(I23/D23)</f>
+        <v>2356.234136318923</v>
+      </c>
+      <c r="J33" s="7">
+        <f>H33/I33</f>
+        <v>0.15701071226222391</v>
+      </c>
+      <c r="L33" s="7">
+        <f>(E33+J33)/2</f>
+        <v>0.13978195187579279</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
       <c r="E39" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>9700</v>
-      </c>
-      <c r="C2">
-        <v>90</v>
-      </c>
-      <c r="D2" s="3">
-        <f>C2/B2</f>
-        <v>9.2783505154639175E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B5" s="1">
+        <f>BoneFlowMale</f>
+        <v>270</v>
+      </c>
+      <c r="C5">
+        <f>SystemicGradient</f>
+        <v>87</v>
+      </c>
+      <c r="D5" s="6">
+        <f>B5/C5</f>
+        <v>3.103448275862069</v>
+      </c>
+      <c r="E5" s="1">
+        <f>BoneMassMale</f>
+        <v>10725</v>
+      </c>
+      <c r="F5" s="4">
+        <f>D5/E5</f>
+        <v>2.8936580660718592E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1300</v>
-      </c>
-      <c r="C3">
-        <v>240</v>
-      </c>
-      <c r="D3" s="3">
-        <f>C3/B3</f>
-        <v>0.18461538461538463</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B6" s="1">
+        <f>BrainFlowMale</f>
+        <v>648</v>
+      </c>
+      <c r="C6">
+        <f>SystemicGradient</f>
+        <v>87</v>
+      </c>
+      <c r="D6" s="6">
+        <f>B6/C6</f>
+        <v>7.4482758620689653</v>
+      </c>
+      <c r="E6" s="1">
+        <f>BrainMassMale</f>
+        <v>1500</v>
+      </c>
+      <c r="F6" s="4">
+        <f>D6/E6</f>
+        <v>4.9655172413793098E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>16600</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4" s="3">
-        <f>C4/B4</f>
-        <v>1.8072289156626507E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B7" s="1">
+        <f>FatFlowMale</f>
+        <v>270</v>
+      </c>
+      <c r="C7">
+        <f>SystemicGradient</f>
+        <v>87</v>
+      </c>
+      <c r="D7" s="6">
+        <f>B7/C7</f>
+        <v>3.103448275862069</v>
+      </c>
+      <c r="E7" s="1">
+        <f>FatMassMale</f>
+        <v>16050</v>
+      </c>
+      <c r="F7" s="4">
+        <f>D7/E7</f>
+        <v>1.9336126329358685E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <f>KidneyFlowMale</f>
+        <v>1026</v>
+      </c>
+      <c r="C8">
+        <f>SystemicGradient</f>
+        <v>87</v>
+      </c>
+      <c r="D8" s="6">
+        <f>B8/C8</f>
+        <v>11.793103448275861</v>
+      </c>
+      <c r="E8" s="1">
+        <f>KidneyMassMale</f>
+        <v>330</v>
+      </c>
+      <c r="F8" s="4">
+        <f>D8/E8</f>
+        <v>3.5736677115987457E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="1">
+        <f>OtherFlowMale</f>
+        <v>431.99999999999989</v>
+      </c>
+      <c r="C9">
+        <f>SystemicGradient</f>
+        <v>87</v>
+      </c>
+      <c r="D9" s="6">
+        <f>B9/C9</f>
+        <v>4.9655172413793087</v>
+      </c>
+      <c r="E9" s="1">
+        <f>OtherMassMale</f>
+        <v>3525</v>
+      </c>
+      <c r="F9" s="4">
+        <f>D9/E9</f>
+        <v>1.4086573734409386E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <f>RMuscleFlowMale</f>
+        <v>110.16000000000001</v>
+      </c>
+      <c r="C10">
+        <f>SystemicGradient</f>
+        <v>87</v>
+      </c>
+      <c r="D10" s="6">
+        <f>B10/C10</f>
+        <v>1.2662068965517244</v>
+      </c>
+      <c r="E10" s="1">
+        <f>RMuscleMassMale</f>
+        <v>3600</v>
+      </c>
+      <c r="F10" s="4">
+        <f>D10/E10</f>
+        <v>3.5172413793103452E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <f>SMuscleFlowMale</f>
+        <v>807.84000000000015</v>
+      </c>
+      <c r="C11">
+        <f>SystemicGradient</f>
+        <v>87</v>
+      </c>
+      <c r="D11" s="6">
+        <f>B11/C11</f>
+        <v>9.2855172413793117</v>
+      </c>
+      <c r="E11" s="1">
+        <f>SMuscleMassMale</f>
+        <v>26400</v>
+      </c>
+      <c r="F11" s="4">
+        <f>D11/E11</f>
+        <v>3.5172413793103452E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <f>SkinFlowMale</f>
+        <v>270</v>
+      </c>
+      <c r="C12">
+        <f>SystemicGradient</f>
+        <v>87</v>
+      </c>
+      <c r="D12" s="6">
+        <f>B12/C12</f>
+        <v>3.103448275862069</v>
+      </c>
+      <c r="E12" s="1">
+        <f>SkinMassMale</f>
+        <v>2775</v>
+      </c>
+      <c r="F12" s="4">
+        <f>D12/E12</f>
+        <v>1.1183597390493941E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="1">
+        <f>SUM(B5:B12)</f>
+        <v>3834</v>
+      </c>
+      <c r="C13">
+        <f>SystemicVeinsGradient</f>
+        <v>8</v>
+      </c>
+      <c r="D13" s="1">
+        <f>B13/C13</f>
+        <v>479.25</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="1">
+        <f>GIFlowMale</f>
+        <v>1026</v>
+      </c>
+      <c r="C15">
+        <f>GITractGradient</f>
+        <v>89</v>
+      </c>
+      <c r="D15" s="6">
+        <f>B15/C15</f>
+        <v>11.52808988764045</v>
+      </c>
+      <c r="E15" s="1">
+        <f>GIMassMale</f>
+        <v>1275</v>
+      </c>
+      <c r="F15" s="4">
+        <f>D15/E15</f>
+        <v>9.0416391275611376E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="1">
+        <f>HepaticArtyFlowMale</f>
+        <v>324</v>
+      </c>
+      <c r="C16">
+        <f>GITractGradient</f>
+        <v>89</v>
+      </c>
+      <c r="D16" s="6">
+        <f>B16/C16</f>
+        <v>3.6404494382022472</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1">
+        <f>SUM(B15:B16)</f>
+        <v>1350</v>
+      </c>
+      <c r="C17">
+        <f>HepaticGradient</f>
+        <v>6</v>
+      </c>
+      <c r="D17" s="1">
+        <f>B17/C17</f>
+        <v>225</v>
+      </c>
+      <c r="E17" s="1">
+        <f>LiverMassMale</f>
+        <v>1950</v>
+      </c>
+      <c r="F17" s="4">
+        <f>D17/E17</f>
+        <v>0.11538461538461539</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" s="1">
+        <f>LiverFlowMale</f>
+        <v>1350</v>
+      </c>
+      <c r="C19">
+        <f>HepaticGradient</f>
+        <v>6</v>
+      </c>
+      <c r="D19" s="1">
+        <f>B19/C19</f>
+        <v>225</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1">
+        <f>LHeartFlowMale</f>
+        <v>179.28</v>
+      </c>
+      <c r="C21">
+        <f>CoronaryGradient</f>
+        <v>95</v>
+      </c>
+      <c r="D21" s="6">
+        <f>B21/C21</f>
+        <v>1.8871578947368421</v>
+      </c>
+      <c r="E21" s="1">
+        <f>LHeartMassMale</f>
+        <v>292.57499999999993</v>
+      </c>
+      <c r="F21" s="4">
+        <f>D21/E21</f>
+        <v>6.4501679731243013E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="1">
+        <f>RHeartFlowMale</f>
+        <v>36.720000000000006</v>
+      </c>
+      <c r="C22">
+        <f>CoronaryGradient</f>
+        <v>95</v>
+      </c>
+      <c r="D22" s="6">
+        <f>B22/C22</f>
+        <v>0.38652631578947377</v>
+      </c>
+      <c r="E22" s="1">
+        <f>RHeartMassMale</f>
+        <v>59.924999999999997</v>
+      </c>
+      <c r="F22" s="4">
+        <f>D22/E22</f>
+        <v>6.4501679731243022E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="1">
+        <f>SUM(B21:B22)</f>
+        <v>216</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="1">
+        <f>SystemicVeinOutflow+HepaticVeinOutflow+CoronarySinusOutflow</f>
+        <v>5400</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27">
+        <f>VenousReturn</f>
+        <v>5400</v>
+      </c>
+      <c r="C27">
+        <f>PulmArtyGradient</f>
+        <v>4</v>
+      </c>
+      <c r="D27" s="1">
+        <f>B27/C27</f>
+        <v>1350</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28">
+        <f>VenousReturn</f>
+        <v>5400</v>
+      </c>
+      <c r="C28">
+        <f>PulmCapysGradient</f>
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>1500</v>
-      </c>
-      <c r="C5">
-        <v>120</v>
-      </c>
-      <c r="D5" s="3">
-        <f>C5/B5</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>290</v>
-      </c>
-      <c r="C6">
-        <v>110</v>
-      </c>
-      <c r="D6" s="3">
-        <f>C6/B6</f>
-        <v>0.37931034482758619</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7">
-        <v>50</v>
-      </c>
-      <c r="D7" s="3">
-        <f>C7/B6</f>
-        <v>0.17241379310344829</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8">
-        <v>60</v>
-      </c>
-      <c r="D8" s="3">
-        <f>C8/B6</f>
-        <v>0.20689655172413793</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>260</v>
-      </c>
-      <c r="C9">
-        <v>130</v>
-      </c>
-      <c r="D9" s="3">
-        <f>C9/B9</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10">
-        <v>20</v>
-      </c>
-      <c r="D10" s="3">
-        <f>C10/B9</f>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11">
-        <v>110</v>
-      </c>
-      <c r="D11" s="3">
-        <f>C11/B9</f>
-        <v>0.42307692307692307</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>1750</v>
-      </c>
-      <c r="C12">
-        <v>190</v>
-      </c>
-      <c r="D12" s="3">
-        <f>C12/B12</f>
-        <v>0.10857142857142857</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>4100</v>
-      </c>
-      <c r="C13">
-        <v>50</v>
-      </c>
-      <c r="D13" s="3">
-        <f>C13/B13</f>
-        <v>1.2195121951219513E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>3500</v>
-      </c>
-      <c r="C14">
-        <v>30</v>
-      </c>
-      <c r="D14" s="3">
-        <f>C14/B14</f>
-        <v>8.5714285714285719E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15">
-        <v>10</v>
-      </c>
-      <c r="D15" s="3">
-        <f>C15/B14</f>
-        <v>2.8571428571428571E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16">
-        <v>20</v>
-      </c>
-      <c r="D16" s="3">
-        <f>C16/B14</f>
-        <v>5.7142857142857143E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <v>50</v>
-      </c>
-      <c r="C17">
-        <v>25</v>
-      </c>
-      <c r="D17" s="3">
-        <f>C17/B17</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18" s="3">
-        <f>C18/B17</f>
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19">
-        <v>22</v>
-      </c>
-      <c r="D19" s="3">
-        <f>C19/B17</f>
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20">
-        <v>27000</v>
-      </c>
-      <c r="C20">
-        <v>140</v>
-      </c>
-      <c r="D20" s="3">
-        <f>C20/B20</f>
-        <v>5.185185185185185E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21">
-        <v>140</v>
-      </c>
-      <c r="D21" s="3">
-        <f>C21/B20</f>
-        <v>5.185185185185185E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22">
-        <v>2550</v>
-      </c>
-      <c r="C22">
-        <v>40</v>
-      </c>
-      <c r="D22" s="3">
-        <f>C22/B22</f>
-        <v>1.5686274509803921E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23">
-        <f>SUM(B2:B22)</f>
-        <v>68600</v>
-      </c>
-      <c r="C23">
-        <f>SUM(C2:C6,C9,C12:C14,C17,C20,C22)</f>
-        <v>1195</v>
-      </c>
+      <c r="D28" s="1">
+        <f>B28/C28</f>
+        <v>1800</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29">
+        <f>VenousReturn</f>
+        <v>5400</v>
+      </c>
+      <c r="C29">
+        <f>PulmVeinsGradient</f>
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <f>B29/C29</f>
+        <v>5400</v>
+      </c>
+      <c r="E29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
HumModRepository - Updated log. New Web pages for Normal Values. Fixed error in the model -- see log.
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -14,14 +14,21 @@
     <sheet name="Pressure Gradients" sheetId="9" r:id="rId5"/>
     <sheet name="Organ Composition" sheetId="1" r:id="rId6"/>
     <sheet name="Organ Blood Flow" sheetId="7" r:id="rId7"/>
-    <sheet name="Systemic Blood Flow" sheetId="10" r:id="rId8"/>
-    <sheet name="Vascular Conductance" sheetId="3" r:id="rId9"/>
-    <sheet name="Calories" sheetId="2" r:id="rId10"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId11"/>
+    <sheet name="Flows &amp; Conductances" sheetId="10" r:id="rId8"/>
+    <sheet name="Cardiac Output" sheetId="13" r:id="rId9"/>
+    <sheet name="Blood Volume" sheetId="12" r:id="rId10"/>
+    <sheet name="Calories Used" sheetId="2" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="AdrenalMassFemale">'Organ Mass - Female'!$D$29</definedName>
     <definedName name="AdrenalMassMale">'Organ Mass - Male'!$C$35</definedName>
+    <definedName name="AfferentArtyGradient">'Pressure Gradients'!$D$8</definedName>
+    <definedName name="ArcuateArtyGradient">'Pressure Gradients'!$D$7</definedName>
+    <definedName name="ArcuateArtyPressure">'Blood Pressures'!$B$7</definedName>
+    <definedName name="BaseFlowFemale">'Organ Blood Flow'!$H$23</definedName>
+    <definedName name="BaseFlowGFemale">'Organ Blood Flow'!$J$23</definedName>
+    <definedName name="BaseFlowGMale">'Organ Blood Flow'!$E$23</definedName>
+    <definedName name="BaseFlowMale">'Organ Blood Flow'!$C$23</definedName>
     <definedName name="BaseMassFemale">'Organ Mass - Female'!$D$16</definedName>
     <definedName name="BaseMassMale">'Organ Mass - Male'!$C$16</definedName>
     <definedName name="BloodMass">'Organ Mass - Male'!$C$19</definedName>
@@ -38,8 +45,11 @@
     <definedName name="CardiacOutputFemale">'Organ Blood Flow'!$D$5</definedName>
     <definedName name="CardiacOutputMale">'Organ Blood Flow'!$D$4</definedName>
     <definedName name="CoronaryGradient">'Pressure Gradients'!$D$6</definedName>
-    <definedName name="CoronarySinusOutflow">'Systemic Blood Flow'!$B$23</definedName>
+    <definedName name="CoronarySinusOutflow">'Flows &amp; Conductances'!$B$30</definedName>
+    <definedName name="EfferentArtyGradient">'Pressure Gradients'!$D$9</definedName>
     <definedName name="FatFlowFemale">'Organ Blood Flow'!$H$9</definedName>
+    <definedName name="FatFlowGFemale">'Organ Blood Flow'!$J$9</definedName>
+    <definedName name="FatFlowGMale">'Organ Blood Flow'!$E$9</definedName>
     <definedName name="FatFlowMale">'Organ Blood Flow'!$C$9</definedName>
     <definedName name="FatMassFemale">'Organ Mass - Female'!$D$6</definedName>
     <definedName name="FatMassMale">'Organ Mass - Male'!$C$6</definedName>
@@ -49,6 +59,7 @@
     <definedName name="GIMassFemale">'Organ Mass - Female'!$D$7</definedName>
     <definedName name="GIMassMale">'Organ Mass - Male'!$C$7</definedName>
     <definedName name="GITractGradient">'Pressure Gradients'!$D$5</definedName>
+    <definedName name="GlomularPressure">'Blood Pressures'!$B$8</definedName>
     <definedName name="GutH2OMass">'Organ Mass - Male'!$C$22</definedName>
     <definedName name="HeartFlowFemale">'Organ Blood Flow'!$H$14</definedName>
     <definedName name="HeartFlowMale">'Organ Blood Flow'!$C$14</definedName>
@@ -57,19 +68,22 @@
     <definedName name="Hematocrit">'Organ Composition'!$B$19</definedName>
     <definedName name="HepaticArtyFlowFemale">'Organ Blood Flow'!$H$15</definedName>
     <definedName name="HepaticArtyFlowMale">'Organ Blood Flow'!$C$15</definedName>
-    <definedName name="HepaticGradient">'Pressure Gradients'!$D$7</definedName>
-    <definedName name="HepaticVeinOutflow">'Systemic Blood Flow'!$B$19</definedName>
+    <definedName name="HepaticGradient">'Pressure Gradients'!$D$14</definedName>
+    <definedName name="HepaticVeinOutflow">'Flows &amp; Conductances'!$B$22</definedName>
     <definedName name="KidneyFlowFemale">'Organ Blood Flow'!$H$16</definedName>
     <definedName name="KidneyFlowMale">'Organ Blood Flow'!$C$16</definedName>
     <definedName name="KidneyMassFemale">'Organ Mass - Female'!$D$8</definedName>
     <definedName name="KidneyMassMale">'Organ Mass - Male'!$C$8</definedName>
-    <definedName name="LeftAtrialPressure">'Blood Pressures'!$B$11</definedName>
+    <definedName name="LeftAtrialPressure">'Blood Pressures'!$B$18</definedName>
     <definedName name="LHeartFlowFemale">'Organ Blood Flow'!$H$27</definedName>
     <definedName name="LHeartFlowMale">'Organ Blood Flow'!$C$27</definedName>
     <definedName name="LHeartFractionFemale">'Organ Mass - Female'!$B$23</definedName>
     <definedName name="LHeartFractionMale">'Organ Mass - Male'!$B$29</definedName>
+    <definedName name="LHeartLargeVesselGradient">'Pressure Gradients'!$D$10</definedName>
+    <definedName name="LHeartLargeVesselPressure">'Blood Pressures'!$B$9</definedName>
     <definedName name="LHeartMassFemale">'Organ Mass - Female'!$D$9</definedName>
     <definedName name="LHeartMassMale">'Organ Mass - Male'!$C$9</definedName>
+    <definedName name="LHeartSmallVesselGradient">'Pressure Gradients'!$D$11</definedName>
     <definedName name="LiverFlowFemale">'Organ Blood Flow'!$H$17</definedName>
     <definedName name="LiverFlowMale">'Organ Blood Flow'!$C$17</definedName>
     <definedName name="LiverMassFemale">'Organ Mass - Female'!$D$10</definedName>
@@ -81,24 +95,29 @@
     <definedName name="MuscleFlowMale">'Organ Blood Flow'!$C$19</definedName>
     <definedName name="MuscleMassFemale">'Organ Mass - Female'!$C$25</definedName>
     <definedName name="MuscleMassMale">'Organ Mass - Male'!$C$31</definedName>
+    <definedName name="OrganMassFemale">'Organ Mass - Female'!$D$17</definedName>
+    <definedName name="OrganMassMale">'Organ Mass - Male'!$C$17</definedName>
     <definedName name="OtherFlowFemale">'Organ Blood Flow'!$H$33</definedName>
     <definedName name="OtherFlowMale">'Organ Blood Flow'!$C$33</definedName>
     <definedName name="OtherMassFemale">'Organ Mass - Female'!$D$11</definedName>
     <definedName name="OtherMassMale">'Organ Mass - Male'!$C$11</definedName>
     <definedName name="PeritoneumMass">'Organ Mass - Male'!$C$21</definedName>
-    <definedName name="PulmArtyGradient">'Pressure Gradients'!$D$9</definedName>
-    <definedName name="PulmArtyPressure">'Blood Pressures'!$B$8</definedName>
-    <definedName name="PulmCapysGradient">'Pressure Gradients'!$D$10</definedName>
-    <definedName name="PulmCapysPressure">'Blood Pressures'!$B$9</definedName>
-    <definedName name="PulmVeinsGradient">'Pressure Gradients'!$D$11</definedName>
-    <definedName name="PulmVeinsPressure">'Blood Pressures'!$B$10</definedName>
+    <definedName name="PulmArtyGradient">'Pressure Gradients'!$D$17</definedName>
+    <definedName name="PulmArtyPressure">'Blood Pressures'!$B$15</definedName>
+    <definedName name="PulmCapysGradient">'Pressure Gradients'!$D$18</definedName>
+    <definedName name="PulmCapysPressure">'Blood Pressures'!$B$16</definedName>
+    <definedName name="PulmVeinsGradient">'Pressure Gradients'!$D$19</definedName>
+    <definedName name="PulmVeinsPressure">'Blood Pressures'!$B$17</definedName>
     <definedName name="RHeartFlowFemale">'Organ Blood Flow'!$H$26</definedName>
     <definedName name="RHeartFlowMale">'Organ Blood Flow'!$C$26</definedName>
     <definedName name="RHeartFractionFemale">'Organ Mass - Female'!$B$22</definedName>
     <definedName name="RHeartFractionMale">'Organ Mass - Male'!$B$28</definedName>
+    <definedName name="RheartLargeVesselGradient">'Pressure Gradients'!$D$12</definedName>
+    <definedName name="RHeartLargeVesselPressure">'Blood Pressures'!$B$10</definedName>
     <definedName name="RHeartMassFemale">'Organ Mass - Female'!$D$13</definedName>
     <definedName name="RHeartMassMale">'Organ Mass - Male'!$C$13</definedName>
-    <definedName name="RightAtrialPressure">'Blood Pressures'!$B$7</definedName>
+    <definedName name="RHeartSmallVesselGradient">'Pressure Gradients'!$D$13</definedName>
+    <definedName name="RightAtrialPressure">'Blood Pressures'!$B$14</definedName>
     <definedName name="RMuscleFlowFemale">'Organ Blood Flow'!$H$30</definedName>
     <definedName name="RMuscleFlowMale">'Organ Blood Flow'!$C$30</definedName>
     <definedName name="RMuscleFractionFemale">'Organ Mass - Female'!$B$26</definedName>
@@ -110,27 +129,29 @@
     <definedName name="SkinMassFemale">'Organ Mass - Female'!$D$15</definedName>
     <definedName name="SkinMassMale">'Organ Mass - Male'!$C$15</definedName>
     <definedName name="SMuscleFlowFemale">'Organ Blood Flow'!$H$31</definedName>
+    <definedName name="SMuscleFlowGFemale">'Organ Blood Flow'!$J$31</definedName>
+    <definedName name="SMuscleFlowGMale">'Organ Blood Flow'!$E$31</definedName>
     <definedName name="SMuscleFlowMale">'Organ Blood Flow'!$C$31</definedName>
     <definedName name="SMuscleFractionFemale">'Organ Mass - Female'!$B$27</definedName>
     <definedName name="SMuscleFractionMale">'Organ Mass - Male'!$B$33</definedName>
     <definedName name="SMuscleMassFemale">'Organ Mass - Female'!$D$14</definedName>
     <definedName name="SMuscleMassMale">'Organ Mass - Male'!$C$14</definedName>
-    <definedName name="SplanchnicVeinsPressure">'Blood Pressures'!$B$6</definedName>
+    <definedName name="SplanchnicVeinsPressure">'Blood Pressures'!$B$13</definedName>
     <definedName name="SystemicArtysPressure">'Blood Pressures'!$B$4</definedName>
     <definedName name="SystemicGradient">'Pressure Gradients'!$D$4</definedName>
-    <definedName name="SystemicVeinOutflow">'Systemic Blood Flow'!$B$13</definedName>
-    <definedName name="SystemicVeinsGradient">'Pressure Gradients'!$D$8</definedName>
-    <definedName name="SystemicVeinsPressure">'Blood Pressures'!$B$5</definedName>
+    <definedName name="SystemicVeinOutflow">'Flows &amp; Conductances'!$B$16</definedName>
+    <definedName name="SystemicVeinsGradient">'Pressure Gradients'!$D$15</definedName>
+    <definedName name="SystemicVeinsPressure">'Blood Pressures'!$B$12</definedName>
     <definedName name="ThyroidMassFemale">'Organ Mass - Female'!$D$36</definedName>
     <definedName name="ThyroidMassMale">'Organ Mass - Male'!$C$42</definedName>
-    <definedName name="VenousReturn">'Systemic Blood Flow'!$B$25</definedName>
+    <definedName name="VenousReturn">'Flows &amp; Conductances'!$B$32</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="146">
   <si>
     <t>Bone</t>
   </si>
@@ -168,9 +189,6 @@
     <t>Skin</t>
   </si>
   <si>
-    <t>Base Mass</t>
-  </si>
-  <si>
     <t>Organ Mass</t>
   </si>
   <si>
@@ -255,21 +273,9 @@
     <t>Hepatic Artery</t>
   </si>
   <si>
-    <t>Portal Vein</t>
-  </si>
-  <si>
-    <t>Hepatic Vein</t>
-  </si>
-  <si>
     <t>Conductance</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Infinite</t>
-  </si>
-  <si>
     <t>Conductance (/G)</t>
   </si>
   <si>
@@ -510,9 +516,6 @@
     <t>Flow (/G)</t>
   </si>
   <si>
-    <t>Systemic Blood Flow</t>
-  </si>
-  <si>
     <t>Organ Blood Flow</t>
   </si>
   <si>
@@ -532,6 +535,60 @@
   </si>
   <si>
     <t>Pullmonary Veins Outflow</t>
+  </si>
+  <si>
+    <t>Arcuate Artery</t>
+  </si>
+  <si>
+    <t>Glomerulus</t>
+  </si>
+  <si>
+    <t>Left Heart Large Vessel</t>
+  </si>
+  <si>
+    <t>Right Heart Large Vessel</t>
+  </si>
+  <si>
+    <t>Kidney Arcuate</t>
+  </si>
+  <si>
+    <t>Kidney Afferent</t>
+  </si>
+  <si>
+    <t>Kidney Efferent</t>
+  </si>
+  <si>
+    <t>Left Heart Small Vessel</t>
+  </si>
+  <si>
+    <t>Right Heart Small Vessel</t>
+  </si>
+  <si>
+    <t>Calories Used</t>
+  </si>
+  <si>
+    <t>Flows &amp; Conductances (Male)</t>
+  </si>
+  <si>
+    <t>Blood Volume</t>
+  </si>
+  <si>
+    <t>Cardiac Output</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Body Mass (kG)</t>
+  </si>
+  <si>
+    <t>Blood (mL/kG)</t>
+  </si>
+  <si>
+    <t>BV (mL)</t>
   </si>
 </sst>
 </file>
@@ -544,10 +601,17 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -573,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -588,6 +652,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,20 +964,20 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B4">
         <v>75</v>
@@ -922,12 +987,12 @@
         <v>165</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B5" s="5">
         <f>E5*BodyMassMale</f>
@@ -949,10 +1014,231 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4">
+        <f>BodyMassMale</f>
+        <v>75</v>
+      </c>
+      <c r="C4">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="D4" s="1">
+        <f>C4*B4</f>
+        <v>5407.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="5">
+        <f>BodyMassFemale</f>
+        <v>60.45</v>
+      </c>
+      <c r="C5">
+        <v>65.5</v>
+      </c>
+      <c r="D5" s="1">
+        <f>C5*B5</f>
+        <v>3959.4750000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="1">
+        <f>BaseMassMale</f>
+        <v>26032.5</v>
+      </c>
+      <c r="C9" s="5">
+        <v>100</v>
+      </c>
+      <c r="D9" s="1">
+        <f>0.001*C9*B9</f>
+        <v>2603.25</v>
+      </c>
+      <c r="F9" s="1">
+        <f>BaseMassFemale</f>
+        <v>20794.799999999996</v>
+      </c>
+      <c r="G9" s="5">
+        <v>100</v>
+      </c>
+      <c r="H9" s="1">
+        <f>0.001*G9*F9</f>
+        <v>2079.4799999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1">
+        <f>SMuscleMassMale</f>
+        <v>26400</v>
+      </c>
+      <c r="C10" s="5">
+        <v>88</v>
+      </c>
+      <c r="D10" s="1">
+        <f>0.001*C10*B10</f>
+        <v>2323.1999999999998</v>
+      </c>
+      <c r="F10" s="1">
+        <f>SMuscleMassFemale</f>
+        <v>14628.900000000001</v>
+      </c>
+      <c r="G10" s="5">
+        <v>88</v>
+      </c>
+      <c r="H10" s="1">
+        <f>0.001*G10*F10</f>
+        <v>1287.3432</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <f>FatMassMale</f>
+        <v>16050</v>
+      </c>
+      <c r="C11" s="5">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1">
+        <f>0.001*C11*B11</f>
+        <v>481.5</v>
+      </c>
+      <c r="F11" s="1">
+        <f>FatMassFemale</f>
+        <v>19767.150000000001</v>
+      </c>
+      <c r="G11" s="5">
+        <v>30</v>
+      </c>
+      <c r="H11" s="1">
+        <f>0.001*G11*F11</f>
+        <v>593.0145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1">
+        <f>SUM(B9:B11)</f>
+        <v>68482.5</v>
+      </c>
+      <c r="D12" s="1">
+        <f>SUM(D9:D11)</f>
+        <v>5407.95</v>
+      </c>
+      <c r="F12" s="1">
+        <f>SUM(F9:F11)</f>
+        <v>55190.85</v>
+      </c>
+      <c r="H12" s="1">
+        <f>SUM(H9:H11)</f>
+        <v>3959.8377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="1">
+        <f>OrganMassMale</f>
+        <v>68482.5</v>
+      </c>
+      <c r="D13" s="1">
+        <f>D4</f>
+        <v>5407.5</v>
+      </c>
+      <c r="F13" s="1">
+        <f>OrganMassFemale</f>
+        <v>55190.85</v>
+      </c>
+      <c r="H13" s="1">
+        <f>D5</f>
+        <v>3959.4750000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,334 +1250,351 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>9700</v>
-      </c>
-      <c r="C2">
-        <v>90</v>
-      </c>
-      <c r="D2" s="3">
-        <f>C2/B2</f>
-        <v>9.2783505154639175E-3</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1300</v>
-      </c>
-      <c r="C3">
-        <v>240</v>
-      </c>
-      <c r="D3" s="3">
-        <f>C3/B3</f>
-        <v>0.18461538461538463</v>
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>16600</v>
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <f>BoneMassMale</f>
+        <v>10725</v>
       </c>
       <c r="C4">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D4" s="3">
         <f>C4/B4</f>
-        <v>1.8072289156626507E-3</v>
+        <v>8.3916083916083916E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <f>BrainMassMale</f>
         <v>1500</v>
       </c>
       <c r="C5">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="D5" s="3">
         <f>C5/B5</f>
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>290</v>
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <f>FatMassMale</f>
+        <v>16050</v>
       </c>
       <c r="C6">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="D6" s="3">
         <f>C6/B6</f>
-        <v>0.37931034482758619</v>
+        <v>1.869158878504673E-3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1500</v>
       </c>
       <c r="C7">
+        <v>120</v>
+      </c>
+      <c r="D7" s="3">
+        <f>C7/B7</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <f>KidneyMassMale</f>
+        <v>330</v>
+      </c>
+      <c r="C8">
+        <v>110</v>
+      </c>
+      <c r="D8" s="3">
+        <f>C8/B8</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9">
         <v>50</v>
       </c>
-      <c r="D7" s="3">
-        <f>C7/B6</f>
-        <v>0.17241379310344829</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8">
-        <v>60</v>
-      </c>
-      <c r="D8" s="3">
-        <f>C8/B6</f>
-        <v>0.20689655172413793</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>260</v>
-      </c>
-      <c r="C9">
-        <v>130</v>
-      </c>
       <c r="D9" s="3">
-        <f>C9/B9</f>
-        <v>0.5</v>
+        <f>C9/B8</f>
+        <v>0.15151515151515152</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="B10" s="1"/>
       <c r="C10">
+        <v>60</v>
+      </c>
+      <c r="D10" s="3">
+        <f>C10/B8</f>
+        <v>0.18181818181818182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1">
+        <f>LHeartMassMale</f>
+        <v>292.57499999999993</v>
+      </c>
+      <c r="C11">
+        <v>130</v>
+      </c>
+      <c r="D11" s="3">
+        <f>C11/B11</f>
+        <v>0.44433051354353598</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12">
         <v>20</v>
       </c>
-      <c r="D10" s="3">
-        <f>C10/B9</f>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11">
+      <c r="D12" s="3">
+        <f>C12/B11</f>
+        <v>6.8358540545159371E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13">
         <v>110</v>
       </c>
-      <c r="D11" s="3">
-        <f>C11/B9</f>
-        <v>0.42307692307692307</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>1750</v>
-      </c>
-      <c r="C12">
-        <v>190</v>
-      </c>
-      <c r="D12" s="3">
-        <f>C12/B12</f>
-        <v>0.10857142857142857</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>4100</v>
-      </c>
-      <c r="C13">
-        <v>50</v>
-      </c>
       <c r="D13" s="3">
-        <f>C13/B13</f>
-        <v>1.2195121951219513E-2</v>
+        <f>C13/B11</f>
+        <v>0.37597197299837659</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>3500</v>
+        <v>6</v>
+      </c>
+      <c r="B14" s="1">
+        <f>LiverMassMale</f>
+        <v>1950</v>
       </c>
       <c r="C14">
-        <v>30</v>
+        <v>190</v>
       </c>
       <c r="D14" s="3">
         <f>C14/B14</f>
-        <v>8.5714285714285719E-3</v>
+        <v>9.7435897435897437E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1">
+        <f>OtherMassMale</f>
+        <v>3525</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15" s="3">
+        <f>C15/B15</f>
+        <v>1.4184397163120567E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1">
+        <f>RMuscleMassMale</f>
+        <v>3600</v>
+      </c>
+      <c r="C16">
         <v>30</v>
       </c>
-      <c r="C15">
+      <c r="D16" s="3">
+        <f>C16/B16</f>
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17">
         <v>10</v>
       </c>
-      <c r="D15" s="3">
-        <f>C15/B14</f>
-        <v>2.8571428571428571E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16">
-        <v>20</v>
-      </c>
-      <c r="D16" s="3">
-        <f>C16/B14</f>
-        <v>5.7142857142857143E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <v>50</v>
-      </c>
-      <c r="C17">
-        <v>25</v>
-      </c>
       <c r="D17" s="3">
-        <f>C17/B17</f>
-        <v>0.5</v>
+        <f>C17/B16</f>
+        <v>2.7777777777777779E-3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B18" s="1"/>
       <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18" s="3">
+        <f>C18/B16</f>
+        <v>5.5555555555555558E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1">
+        <f>RHeartMassMale</f>
+        <v>59.924999999999997</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+      <c r="D19" s="3">
+        <f>C19/B19</f>
+        <v>0.41718815185648728</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20">
         <v>3</v>
       </c>
-      <c r="D18" s="3">
-        <f>C18/B17</f>
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19">
-        <v>22</v>
-      </c>
-      <c r="D19" s="3">
-        <f>C19/B17</f>
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20">
-        <v>27000</v>
-      </c>
-      <c r="C20">
-        <v>140</v>
-      </c>
       <c r="D20" s="3">
-        <f>C20/B20</f>
-        <v>5.185185185185185E-3</v>
+        <f>C20/B19</f>
+        <v>5.0062578222778473E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B21" s="1"/>
       <c r="C21">
-        <v>140</v>
+        <v>22</v>
       </c>
       <c r="D21" s="3">
-        <f>C21/B20</f>
-        <v>5.185185185185185E-3</v>
+        <f>C21/B19</f>
+        <v>0.36712557363370885</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22">
-        <v>2550</v>
+        <v>10</v>
+      </c>
+      <c r="B22" s="1">
+        <f>SMuscleMassMale</f>
+        <v>26400</v>
       </c>
       <c r="C22">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="D22" s="3">
         <f>C22/B22</f>
-        <v>1.5686274509803921E-2</v>
+        <v>5.3030303030303034E-3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23">
-        <f>SUM(B2:B22)</f>
-        <v>68600</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B23" s="1"/>
       <c r="C23">
-        <f>SUM(C2:C6,C9,C12:C14,C17,C20,C22)</f>
+        <v>140</v>
+      </c>
+      <c r="D23" s="3">
+        <f>C23/B22</f>
+        <v>5.3030303030303034E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="1">
+        <f>SkinMassMale</f>
+        <v>2775</v>
+      </c>
+      <c r="C24">
+        <v>40</v>
+      </c>
+      <c r="D24" s="3">
+        <f>C24/B24</f>
+        <v>1.4414414414414415E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1">
+        <f>SUM(B4:B24)</f>
+        <v>68707.5</v>
+      </c>
+      <c r="C25">
+        <f>SUM(C4:C8,C11,C14:C16,C19,C22,C24)</f>
         <v>1195</v>
+      </c>
+      <c r="D25" s="3">
+        <f>C25/B25</f>
+        <v>1.739256995233417E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1300,7 +1603,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,21 +1615,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1376,7 +1679,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>1.7</v>
@@ -1521,7 +1824,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B16" s="5">
         <f>SUM(B4:B5,B7:B13,B15)</f>
@@ -1534,7 +1837,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B17" s="5">
         <f>SUM(B4:B15)</f>
@@ -1551,7 +1854,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="5">
         <v>7.4</v>
@@ -1563,7 +1866,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="5">
         <v>0</v>
@@ -1575,7 +1878,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="5">
         <v>0</v>
@@ -1587,7 +1890,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B22" s="5">
         <v>1.3</v>
@@ -1599,7 +1902,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B23">
         <v>8.6999999999999993</v>
@@ -1614,7 +1917,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B25" s="5">
         <f>B17+B23</f>
@@ -1631,7 +1934,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>0.47</v>
@@ -1643,7 +1946,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B28">
         <v>0.17</v>
@@ -1655,7 +1958,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B29">
         <f>1-RHeartFractionMale</f>
@@ -1668,7 +1971,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B31">
         <v>40</v>
@@ -1680,7 +1983,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B32">
         <v>0.12</v>
@@ -1692,7 +1995,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B33">
         <f>1-RMuscleFractionMale</f>
@@ -1708,7 +2011,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B35">
         <v>0.02</v>
@@ -1720,7 +2023,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B36">
         <v>0.21</v>
@@ -1732,7 +2035,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B37">
         <v>0.91</v>
@@ -1744,7 +2047,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B38">
         <v>0.53</v>
@@ -1756,7 +2059,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B39">
         <v>0.76</v>
@@ -1768,7 +2071,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B40">
         <v>0.14000000000000001</v>
@@ -1780,7 +2083,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B41">
         <v>0.26</v>
@@ -1792,7 +2095,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B42">
         <v>0.03</v>
@@ -1813,7 +2116,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,21 +2129,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1884,7 +2187,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C7" s="5">
         <f>'Organ Mass - Male'!D7</f>
@@ -2001,7 +2304,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C16" s="5">
         <f>SUM(C4:C5,C7:C13,C15)</f>
@@ -2014,7 +2317,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D17" s="1">
         <f>SUM(D4:D15)</f>
@@ -2023,7 +2326,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B18">
         <v>8.6999999999999993</v>
@@ -2035,7 +2338,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19" s="1">
         <f>D17+D18</f>
@@ -2047,7 +2350,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B21" s="6">
         <f>100*C21/D16</f>
@@ -2061,7 +2364,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B22">
         <f>C22/C21</f>
@@ -2075,7 +2378,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B23">
         <f>C23/C21</f>
@@ -2093,7 +2396,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B25" s="5">
         <f>0.1*MuscleMassFemale/BodyMassFemale</f>
@@ -2107,7 +2410,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B26" s="6">
         <f>RMuscleMassFemale/MuscleMassFemale</f>
@@ -2121,7 +2424,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B27" s="6">
         <f>SMuscleMassFemale/MuscleMassFemale</f>
@@ -2135,7 +2438,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B29">
         <v>0.02</v>
@@ -2147,7 +2450,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B30">
         <v>0.21</v>
@@ -2159,7 +2462,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B31">
         <v>0.91</v>
@@ -2171,7 +2474,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B32">
         <v>0.53</v>
@@ -2183,7 +2486,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B33">
         <v>0.76</v>
@@ -2195,7 +2498,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B34">
         <v>0.14000000000000001</v>
@@ -2207,7 +2510,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B35">
         <v>0.26</v>
@@ -2219,7 +2522,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B36">
         <v>0.03</v>
@@ -2237,45 +2540,46 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B4">
         <v>97</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" ref="C4:C11" si="0">0.1333*B4</f>
+        <f t="shared" ref="C4:C18" si="0">0.1333*B4</f>
         <v>12.930099999999999</v>
       </c>
       <c r="D4">
@@ -2284,211 +2588,290 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5">
-        <f t="shared" si="0"/>
-        <v>1.333</v>
-      </c>
-      <c r="D5">
-        <f>B5</f>
-        <v>10</v>
-      </c>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5">
-        <f t="shared" si="0"/>
-        <v>1.0664</v>
-      </c>
-      <c r="D6">
-        <f>B6</f>
-        <v>8</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>75</v>
+      <c r="A7" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <f>SystemicArtysPressure-2</f>
+        <v>95</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="0"/>
-        <v>0.2666</v>
+        <f>0.1333*B7</f>
+        <v>12.663500000000001</v>
       </c>
       <c r="D7">
-        <f>B7-B21</f>
-        <v>6</v>
+        <f>B7</f>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>76</v>
+      <c r="A8" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="0"/>
-        <v>1.8662000000000001</v>
+        <f>0.1333*B8</f>
+        <v>7.9980000000000002</v>
       </c>
       <c r="D8">
-        <f>B8-B21</f>
-        <v>18</v>
+        <f>B8</f>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <f>SystemicArtysPressure-3.5</f>
+        <v>93.5</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="0"/>
-        <v>1.333</v>
+        <f>0.1333*B9</f>
+        <v>12.46355</v>
       </c>
       <c r="D9">
-        <f>B9-B21</f>
-        <v>14</v>
+        <f>B9-B28</f>
+        <v>97.5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>131</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <f>SystemicArtysPressure-3.5</f>
+        <v>93.5</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="0"/>
-        <v>0.93310000000000004</v>
+        <f>0.1333*B10</f>
+        <v>12.46355</v>
       </c>
       <c r="D10">
-        <f>B10-B21</f>
-        <v>11</v>
+        <f>B10-B28</f>
+        <v>97.5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11">
-        <v>6</v>
-      </c>
-      <c r="C11" s="5">
-        <f t="shared" si="0"/>
-        <v>0.79980000000000007</v>
-      </c>
-      <c r="D11">
-        <f>B11-B21</f>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="5"/>
+      <c r="C12" s="5">
+        <f t="shared" si="0"/>
+        <v>1.333</v>
+      </c>
+      <c r="D12">
+        <f>B12</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0664</v>
+      </c>
+      <c r="D13">
+        <f>B13</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2666</v>
+      </c>
+      <c r="D14">
+        <f>B14-B28</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="0"/>
+        <v>1.8662000000000001</v>
+      </c>
+      <c r="D15">
+        <f>B15-B28</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14">
-        <v>120</v>
-      </c>
-      <c r="C14" s="5">
-        <f>0.1333*B14</f>
-        <v>15.996</v>
-      </c>
-      <c r="D14">
-        <f>B14</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15">
-        <v>80</v>
-      </c>
-      <c r="C15" s="5">
-        <f>0.1333*B15</f>
-        <v>10.664</v>
-      </c>
-      <c r="D15">
-        <f>B15</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" si="0"/>
+        <v>1.333</v>
+      </c>
+      <c r="D16">
+        <f>B16-B28</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.93310000000000004</v>
+      </c>
+      <c r="D17">
+        <f>B17-B28</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>80</v>
+      <c r="A18" t="s">
+        <v>74</v>
       </c>
       <c r="B18">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C18" s="5">
-        <f>0.1333*B18</f>
-        <v>2.7993000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.79980000000000007</v>
       </c>
       <c r="D18">
-        <f>B18-B21</f>
-        <v>25</v>
+        <f>B18-B28</f>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19">
-        <v>9</v>
-      </c>
-      <c r="C19" s="5">
-        <f>0.1333*B19</f>
-        <v>1.1997</v>
-      </c>
-      <c r="D19">
-        <f>B19-B21</f>
-        <v>13</v>
-      </c>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>82</v>
+      <c r="A21" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="B21">
-        <v>-4</v>
+        <v>120</v>
       </c>
       <c r="C21" s="5">
         <f>0.1333*B21</f>
+        <v>15.996</v>
+      </c>
+      <c r="D21">
+        <f>B21</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22">
+        <v>80</v>
+      </c>
+      <c r="C22" s="5">
+        <f>0.1333*B22</f>
+        <v>10.664</v>
+      </c>
+      <c r="D22">
+        <f>B22</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25">
+        <v>21</v>
+      </c>
+      <c r="C25" s="5">
+        <f>0.1333*B25</f>
+        <v>2.7993000000000001</v>
+      </c>
+      <c r="D25">
+        <f>B25-B28</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="C26" s="5">
+        <f>0.1333*B26</f>
+        <v>1.1997</v>
+      </c>
+      <c r="D26">
+        <f>B26-B28</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28">
+        <v>-4</v>
+      </c>
+      <c r="C28" s="5">
+        <f>0.1333*B28</f>
         <v>-0.53320000000000001</v>
       </c>
     </row>
@@ -2500,10 +2883,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2516,34 +2899,34 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B4">
         <f>SystemicArtysPressure</f>
@@ -2554,13 +2937,13 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D11" si="0">B4-C4</f>
+        <f t="shared" ref="D4:D19" si="0">B4-C4</f>
         <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B5">
         <f>SystemicArtysPressure</f>
@@ -2577,7 +2960,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B6">
         <f>SystemicArtysPressure</f>
@@ -2594,85 +2977,204 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="B7">
+        <f>SystemicArtysPressure</f>
+        <v>97</v>
+      </c>
+      <c r="C7">
+        <f>ArcuateArtyPressure</f>
+        <v>95</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <f>ArcuateArtyPressure</f>
+        <v>95</v>
+      </c>
+      <c r="C8">
+        <f>GlomularPressure</f>
+        <v>60</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9">
+        <f>GlomularPressure</f>
+        <v>60</v>
+      </c>
+      <c r="C9">
+        <f>SystemicVeinsPressure</f>
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10">
+        <f>SystemicArtysPressure</f>
+        <v>97</v>
+      </c>
+      <c r="C10">
+        <f>LHeartLargeVesselPressure</f>
+        <v>93.5</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11">
+        <f>LHeartLargeVesselPressure</f>
+        <v>93.5</v>
+      </c>
+      <c r="C11">
+        <f>RightAtrialPressure</f>
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>91.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12">
+        <f>SystemicArtysPressure</f>
+        <v>97</v>
+      </c>
+      <c r="C12">
+        <f>RHeartLargeVesselPressure</f>
+        <v>93.5</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13">
+        <f>RHeartLargeVesselPressure</f>
+        <v>93.5</v>
+      </c>
+      <c r="C13">
+        <f>RightAtrialPressure</f>
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>91.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14">
         <f>SplanchnicVeinsPressure</f>
         <v>8</v>
       </c>
-      <c r="C7">
+      <c r="C14">
         <f>RightAtrialPressure</f>
         <v>2</v>
       </c>
-      <c r="D7">
+      <c r="D14">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15">
         <f>SystemicVeinsPressure</f>
         <v>10</v>
       </c>
-      <c r="C8">
+      <c r="C15">
         <f>RightAtrialPressure</f>
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17">
         <f>PulmArtyPressure</f>
         <v>14</v>
       </c>
-      <c r="C9">
+      <c r="C17">
         <f>PulmCapysPressure</f>
         <v>10</v>
       </c>
-      <c r="D9">
+      <c r="D17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18">
         <f>PulmCapysPressure</f>
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="C18">
         <f>PulmVeinsPressure</f>
         <v>7</v>
       </c>
-      <c r="D10">
+      <c r="D18">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19">
         <f>PulmVeinsPressure</f>
         <v>7</v>
       </c>
-      <c r="C11">
+      <c r="C19">
         <f>LeftAtrialPressure</f>
         <v>6</v>
       </c>
-      <c r="D11">
+      <c r="D19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2705,59 +3207,59 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2787,7 +3289,7 @@
         <v>5542.68</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I4" s="1">
         <f>E4-G4</f>
@@ -2842,7 +3344,7 @@
         <v>12141.825000000001</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I6" s="1">
         <f>E6-G6</f>
@@ -2918,7 +3420,7 @@
         <v>67.584824999999967</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I9" s="1">
         <f>E9-G9</f>
@@ -2994,7 +3496,7 @@
         <v>378</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I12" s="1">
         <f>E12-G12</f>
@@ -3028,7 +3530,7 @@
         <v>13.842675</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I13" s="1">
         <f>E13-G13</f>
@@ -3062,7 +3564,7 @@
         <v>2772</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I14" s="1">
         <f>E14-G14</f>
@@ -3091,7 +3593,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1">
         <f>SUM(B4:B15)</f>
@@ -3108,7 +3610,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <f>BloodMass</f>
@@ -3117,7 +3619,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B19">
         <v>0.44</v>
@@ -3125,7 +3627,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <f>B18*(1-Hematocrit)</f>
@@ -3134,7 +3636,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <f>B18*Hematocrit</f>
@@ -3146,7 +3648,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1">
         <f>B21*C21</f>
@@ -3155,7 +3657,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
         <f>B21*(1-C21)</f>
@@ -3164,7 +3666,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24">
         <f>LungH2OMass</f>
@@ -3173,7 +3675,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25">
         <f>PeritoneumMass</f>
@@ -3182,7 +3684,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26">
         <f>GutH2OMass</f>
@@ -3191,7 +3693,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B27">
         <f>FluidsMass</f>
@@ -3200,7 +3702,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1">
         <f>B16+B27</f>
@@ -3218,7 +3720,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3235,26 +3737,26 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B4">
         <f>BodyMassMale</f>
@@ -3270,7 +3772,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B5" s="5">
         <f>BodyMassFemale</f>
@@ -3287,50 +3789,50 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" t="s">
         <v>87</v>
-      </c>
-      <c r="G7" t="s">
-        <v>88</v>
-      </c>
-      <c r="L7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="L8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -3351,7 +3853,7 @@
         <v>8.5</v>
       </c>
       <c r="H9" s="1">
-        <f>0.01*G9*CardiacOutputFemale</f>
+        <f t="shared" ref="H9:H21" si="1">0.01*G9*CardiacOutputFemale</f>
         <v>369.95400000000006</v>
       </c>
       <c r="I9" s="1">
@@ -3359,17 +3861,17 @@
         <v>19767.150000000001</v>
       </c>
       <c r="J9" s="7">
-        <f t="shared" ref="J9:J13" si="1">H9/I9</f>
+        <f t="shared" ref="J9:J13" si="2">H9/I9</f>
         <v>1.8715596330275232E-2</v>
       </c>
       <c r="L9" s="7">
-        <f>(E9+J9)/2</f>
+        <f t="shared" ref="L9:L14" si="3">(E9+J9)/2</f>
         <v>1.7769013118408644E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B10">
         <v>0.3</v>
@@ -3390,7 +3892,7 @@
         <v>0.3</v>
       </c>
       <c r="H10" s="1">
-        <f>0.01*G10*CardiacOutputFemale</f>
+        <f t="shared" si="1"/>
         <v>13.057200000000002</v>
       </c>
       <c r="I10" s="1">
@@ -3398,11 +3900,11 @@
         <v>12.090000000000002</v>
       </c>
       <c r="J10" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.08</v>
       </c>
       <c r="L10" s="7">
-        <f>(E10+J10)/2</f>
+        <f t="shared" si="3"/>
         <v>1.08</v>
       </c>
     </row>
@@ -3429,7 +3931,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="1">
-        <f>0.01*G11*CardiacOutputFemale</f>
+        <f t="shared" si="1"/>
         <v>217.62000000000003</v>
       </c>
       <c r="I11" s="1">
@@ -3437,11 +3939,11 @@
         <v>8567.1460674157297</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5401691331923895E-2</v>
       </c>
       <c r="L11" s="7">
-        <f>(E11+J11)/2</f>
+        <f t="shared" si="3"/>
         <v>2.5288258253374538E-2</v>
       </c>
     </row>
@@ -3468,7 +3970,7 @@
         <v>12</v>
       </c>
       <c r="H12" s="1">
-        <f>0.01*G12*CardiacOutputFemale</f>
+        <f t="shared" si="1"/>
         <v>522.28800000000001</v>
       </c>
       <c r="I12" s="1">
@@ -3476,17 +3978,17 @@
         <v>1198.2022471910109</v>
       </c>
       <c r="J12" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.43589302325581408</v>
       </c>
       <c r="L12" s="7">
-        <f>(E12+J12)/2</f>
+        <f t="shared" si="3"/>
         <v>0.43394651162790704</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>19</v>
@@ -3507,7 +4009,7 @@
         <v>21</v>
       </c>
       <c r="H13" s="1">
-        <f>0.01*G13*CardiacOutputFemale</f>
+        <f t="shared" si="1"/>
         <v>914.00400000000013</v>
       </c>
       <c r="I13" s="1">
@@ -3515,17 +4017,17 @@
         <v>1018.4719101123592</v>
       </c>
       <c r="J13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.89742681258549972</v>
       </c>
       <c r="L13" s="7">
-        <f>(E13+J13)/2</f>
+        <f t="shared" si="3"/>
         <v>0.85106634746922039</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -3546,7 +4048,7 @@
         <v>5</v>
       </c>
       <c r="H14" s="1">
-        <f>0.01*G14*CardiacOutputFemale</f>
+        <f t="shared" si="1"/>
         <v>217.62000000000003</v>
       </c>
       <c r="I14" s="1">
@@ -3554,17 +4056,17 @@
         <v>281.57752808988755</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" ref="J14" si="2">H14/I14</f>
+        <f t="shared" ref="J14" si="4">H14/I14</f>
         <v>0.77285997031172726</v>
       </c>
       <c r="L14" s="7">
-        <f>(E14+J14)/2</f>
+        <f t="shared" si="3"/>
         <v>0.69281296387926794</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15">
         <v>6</v>
@@ -3579,7 +4081,7 @@
         <v>6</v>
       </c>
       <c r="H15" s="1">
-        <f>0.01*G15*CardiacOutputFemale</f>
+        <f t="shared" si="1"/>
         <v>261.14400000000001</v>
       </c>
       <c r="I15" s="1"/>
@@ -3609,7 +4111,7 @@
         <v>17</v>
       </c>
       <c r="H16" s="1">
-        <f>0.01*G16*CardiacOutputFemale</f>
+        <f t="shared" si="1"/>
         <v>739.90800000000013</v>
       </c>
       <c r="I16" s="1">
@@ -3617,11 +4119,11 @@
         <v>263.60449438202244</v>
       </c>
       <c r="J16" s="7">
-        <f t="shared" ref="J16:J17" si="3">H16/I16</f>
+        <f t="shared" ref="J16:J17" si="5">H16/I16</f>
         <v>2.8068868921775909</v>
       </c>
       <c r="L16" s="7">
-        <f>(E16+J16)/2</f>
+        <f t="shared" ref="L16:L21" si="6">(E16+J16)/2</f>
         <v>2.9579889006342501</v>
       </c>
     </row>
@@ -3648,7 +4150,7 @@
         <v>27</v>
       </c>
       <c r="H17" s="1">
-        <f>0.01*G17*CardiacOutputFemale</f>
+        <f t="shared" si="1"/>
         <v>1175.1480000000001</v>
       </c>
       <c r="I17" s="1">
@@ -3656,17 +4158,17 @@
         <v>1557.6629213483143</v>
       </c>
       <c r="J17" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.75443023255813979</v>
       </c>
       <c r="L17" s="7">
-        <f>(E17+J17)/2</f>
+        <f t="shared" si="6"/>
         <v>0.72336896243291604</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B18">
         <v>2.5</v>
@@ -3687,7 +4189,7 @@
         <v>2.5</v>
       </c>
       <c r="H18" s="1">
-        <f>0.01*G18*CardiacOutputFemale</f>
+        <f t="shared" si="1"/>
         <v>108.81000000000002</v>
       </c>
       <c r="I18" s="1">
@@ -3699,13 +4201,13 @@
         <v>0.23684210526315791</v>
       </c>
       <c r="L18" s="7">
-        <f>(E18+J18)/2</f>
+        <f t="shared" si="6"/>
         <v>0.23684210526315791</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B19">
         <v>17</v>
@@ -3726,7 +4228,7 @@
         <v>12</v>
       </c>
       <c r="H19" s="1">
-        <f>0.01*G19*CardiacOutputFemale</f>
+        <f t="shared" si="1"/>
         <v>522.28800000000001</v>
       </c>
       <c r="I19" s="1">
@@ -3738,7 +4240,7 @@
         <v>2.9837210551764894E-2</v>
       </c>
       <c r="L19" s="7">
-        <f>(E19+J19)/2</f>
+        <f t="shared" si="6"/>
         <v>3.0218605275882448E-2</v>
       </c>
     </row>
@@ -3765,7 +4267,7 @@
         <v>5</v>
       </c>
       <c r="H20" s="1">
-        <f>0.01*G20*CardiacOutputFemale</f>
+        <f t="shared" si="1"/>
         <v>217.62000000000003</v>
       </c>
       <c r="I20" s="1">
@@ -3777,13 +4279,13 @@
         <v>9.8174104336895066E-2</v>
       </c>
       <c r="L20" s="7">
-        <f>(E20+J20)/2</f>
+        <f t="shared" si="6"/>
         <v>9.7735700817096177E-2</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>1.5</v>
@@ -3804,7 +4306,7 @@
         <v>1.5</v>
       </c>
       <c r="H21" s="1">
-        <f>0.01*G21*CardiacOutputFemale</f>
+        <f t="shared" si="1"/>
         <v>65.286000000000001</v>
       </c>
       <c r="I21" s="1">
@@ -3816,7 +4318,7 @@
         <v>3.5999999999999996</v>
       </c>
       <c r="L21" s="7">
-        <f>(E21+J21)/2</f>
+        <f t="shared" si="6"/>
         <v>3.5999999999999996</v>
       </c>
     </row>
@@ -3831,35 +4333,35 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C23" s="1">
-        <f>SUM(C10:C12,C14,C16:C18,C20:C21)</f>
-        <v>4012.2</v>
+        <f>SUM(BoneFlowMale,BrainFlowMale,KidneyFlowMale,LiverFlowMale,SkinFlowMale,RHeartFlowMale,LHeartFlowMale,RMuscleFlowMale,OtherFlowMale)</f>
+        <v>4322.16</v>
       </c>
       <c r="D23" s="1">
-        <f>SUM(D10:D17,D18:D19,D20:D21)</f>
-        <v>49515</v>
+        <f>BaseMassMale</f>
+        <v>26032.5</v>
       </c>
       <c r="E23" s="7">
         <f>C23/D23</f>
-        <v>8.1029990911844887E-2</v>
+        <v>0.16602938634399309</v>
       </c>
       <c r="H23" s="1">
-        <f>SUM(H10:H12,H14,H16:H18,H20:H21)</f>
-        <v>3277.3572000000004</v>
+        <f>SUM(BoneFlowFemale,BrainFlowFemale,KidneyFlowFemale,LiverFlowFemale,SkinFlowFemale,RHeartFlowFemale,LHeartFlowFemale,RMuscleFlowFemale,OtherFlowFemale)</f>
+        <v>3545.9604305592875</v>
       </c>
       <c r="I23" s="1">
-        <f>SUM(I10:I17,I18:I19,I20:I21)</f>
-        <v>33097.569719101128</v>
+        <f>BaseMassFemale</f>
+        <v>20794.799999999996</v>
       </c>
       <c r="J23" s="7">
         <f>H23/I23</f>
-        <v>9.9021083052771269E-2</v>
+        <v>0.17052149722811896</v>
       </c>
       <c r="L23" s="7">
         <f>(E23+J23)/2</f>
-        <v>9.0025536982308085E-2</v>
+        <v>0.16827544178605602</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -3868,7 +4370,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C25" s="1">
         <f>HeartFlowMale</f>
@@ -3890,7 +4392,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B26">
         <f>RHeartFractionMale</f>
@@ -3931,7 +4433,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B27">
         <f>LHeartFractionMale</f>
@@ -3979,7 +4481,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C29" s="1">
         <f>MuscleFlowMale</f>
@@ -4001,7 +4503,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B30">
         <f>RMuscleFractionMale</f>
@@ -4042,7 +4544,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B31">
         <f>SMuscleFractionMale</f>
@@ -4107,15 +4609,15 @@
       </c>
       <c r="I33" s="1">
         <f>D33*(I23/D23)</f>
-        <v>2356.234136318923</v>
+        <v>2815.7752808988757</v>
       </c>
       <c r="J33" s="7">
         <f>H33/I33</f>
-        <v>0.15701071226222391</v>
+        <v>0.13138619495299361</v>
       </c>
       <c r="L33" s="7">
         <f>(E33+J33)/2</f>
-        <v>0.13978195187579279</v>
+        <v>0.12696969322117763</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -4157,10 +4659,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4173,27 +4675,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4205,11 +4707,11 @@
         <v>270</v>
       </c>
       <c r="C5">
-        <f>SystemicGradient</f>
+        <f t="shared" ref="C5:C15" si="0">SystemicGradient</f>
         <v>87</v>
       </c>
       <c r="D5" s="6">
-        <f>B5/C5</f>
+        <f t="shared" ref="D5:D16" si="1">B5/C5</f>
         <v>3.103448275862069</v>
       </c>
       <c r="E5" s="1">
@@ -4217,7 +4719,7 @@
         <v>10725</v>
       </c>
       <c r="F5" s="4">
-        <f>D5/E5</f>
+        <f t="shared" ref="F5:F15" si="2">D5/E5</f>
         <v>2.8936580660718592E-4</v>
       </c>
     </row>
@@ -4230,11 +4732,11 @@
         <v>648</v>
       </c>
       <c r="C6">
-        <f>SystemicGradient</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
       <c r="D6" s="6">
-        <f>B6/C6</f>
+        <f t="shared" si="1"/>
         <v>7.4482758620689653</v>
       </c>
       <c r="E6" s="1">
@@ -4242,7 +4744,7 @@
         <v>1500</v>
       </c>
       <c r="F6" s="4">
-        <f>D6/E6</f>
+        <f t="shared" si="2"/>
         <v>4.9655172413793098E-3</v>
       </c>
     </row>
@@ -4255,11 +4757,11 @@
         <v>270</v>
       </c>
       <c r="C7">
-        <f>SystemicGradient</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
       <c r="D7" s="6">
-        <f>B7/C7</f>
+        <f t="shared" si="1"/>
         <v>3.103448275862069</v>
       </c>
       <c r="E7" s="1">
@@ -4267,7 +4769,7 @@
         <v>16050</v>
       </c>
       <c r="F7" s="4">
-        <f>D7/E7</f>
+        <f t="shared" si="2"/>
         <v>1.9336126329358685E-4</v>
       </c>
     </row>
@@ -4280,11 +4782,11 @@
         <v>1026</v>
       </c>
       <c r="C8">
-        <f>SystemicGradient</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
       <c r="D8" s="6">
-        <f>B8/C8</f>
+        <f t="shared" si="1"/>
         <v>11.793103448275861</v>
       </c>
       <c r="E8" s="1">
@@ -4292,362 +4794,495 @@
         <v>330</v>
       </c>
       <c r="F8" s="4">
-        <f>D8/E8</f>
+        <f t="shared" si="2"/>
         <v>3.5736677115987457E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9">
+        <f>ArcuateArtyGradient</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <f>KidneyFlowMale/ArcuateArtyGradient</f>
+        <v>513</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="7">
+        <f>D9/E8</f>
+        <v>1.5545454545454545</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10">
+        <f>AfferentArtyGradient</f>
+        <v>35</v>
+      </c>
+      <c r="D10" s="5">
+        <f>KidneyFlowMale/AfferentArtyGradient</f>
+        <v>29.314285714285713</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="4">
+        <f>D10/E8</f>
+        <v>8.883116883116883E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11">
+        <f>EfferentArtyGradient</f>
+        <v>50</v>
+      </c>
+      <c r="D11" s="5">
+        <f>KidneyFlowMale/EfferentArtyGradient</f>
+        <v>20.52</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="4">
+        <f>D11/E8</f>
+        <v>6.2181818181818178E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="1">
         <f>OtherFlowMale</f>
         <v>431.99999999999989</v>
       </c>
-      <c r="C9">
-        <f>SystemicGradient</f>
+      <c r="C12">
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="D9" s="6">
-        <f>B9/C9</f>
+      <c r="D12" s="6">
+        <f t="shared" si="1"/>
         <v>4.9655172413793087</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E12" s="1">
         <f>OtherMassMale</f>
         <v>3525</v>
       </c>
-      <c r="F9" s="4">
-        <f>D9/E9</f>
+      <c r="F12" s="4">
+        <f t="shared" si="2"/>
         <v>1.4086573734409386E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B13" s="1">
         <f>RMuscleFlowMale</f>
         <v>110.16000000000001</v>
       </c>
-      <c r="C10">
-        <f>SystemicGradient</f>
+      <c r="C13">
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="D10" s="6">
-        <f>B10/C10</f>
+      <c r="D13" s="6">
+        <f t="shared" si="1"/>
         <v>1.2662068965517244</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E13" s="1">
         <f>RMuscleMassMale</f>
         <v>3600</v>
       </c>
-      <c r="F10" s="4">
-        <f>D10/E10</f>
+      <c r="F13" s="4">
+        <f t="shared" si="2"/>
         <v>3.5172413793103452E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B14" s="1">
         <f>SMuscleFlowMale</f>
         <v>807.84000000000015</v>
       </c>
-      <c r="C11">
-        <f>SystemicGradient</f>
+      <c r="C14">
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="D11" s="6">
-        <f>B11/C11</f>
+      <c r="D14" s="6">
+        <f t="shared" si="1"/>
         <v>9.2855172413793117</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E14" s="1">
         <f>SMuscleMassMale</f>
         <v>26400</v>
       </c>
-      <c r="F11" s="4">
-        <f>D11/E11</f>
+      <c r="F14" s="4">
+        <f t="shared" si="2"/>
         <v>3.5172413793103452E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B15" s="1">
         <f>SkinFlowMale</f>
         <v>270</v>
       </c>
-      <c r="C12">
-        <f>SystemicGradient</f>
+      <c r="C15">
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
-      <c r="D12" s="6">
-        <f>B12/C12</f>
+      <c r="D15" s="6">
+        <f t="shared" si="1"/>
         <v>3.103448275862069</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E15" s="1">
         <f>SkinMassMale</f>
         <v>2775</v>
       </c>
-      <c r="F12" s="4">
-        <f>D12/E12</f>
+      <c r="F15" s="4">
+        <f t="shared" si="2"/>
         <v>1.1183597390493941E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B13" s="1">
-        <f>SUM(B5:B12)</f>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="1">
+        <f>SUM(B5:B15)</f>
         <v>3834</v>
       </c>
-      <c r="C13">
+      <c r="C16">
         <f>SystemicVeinsGradient</f>
         <v>8</v>
       </c>
-      <c r="D13" s="1">
-        <f>B13/C13</f>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
         <v>479.25</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="E16" s="1"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="1">
         <f>GIFlowMale</f>
         <v>1026</v>
       </c>
-      <c r="C15">
+      <c r="C18">
         <f>GITractGradient</f>
         <v>89</v>
       </c>
-      <c r="D15" s="6">
-        <f>B15/C15</f>
+      <c r="D18" s="6">
+        <f>B18/C18</f>
         <v>11.52808988764045</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E18" s="1">
         <f>GIMassMale</f>
         <v>1275</v>
       </c>
-      <c r="F15" s="4">
-        <f>D15/E15</f>
+      <c r="F18" s="4">
+        <f>D18/E18</f>
         <v>9.0416391275611376E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="1">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1">
         <f>HepaticArtyFlowMale</f>
         <v>324</v>
       </c>
-      <c r="C16">
+      <c r="C19">
         <f>GITractGradient</f>
         <v>89</v>
       </c>
-      <c r="D16" s="6">
-        <f>B16/C16</f>
+      <c r="D19" s="6">
+        <f>B19/C19</f>
         <v>3.6404494382022472</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E19" s="1"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="1">
-        <f>SUM(B15:B16)</f>
+      <c r="B20" s="1">
+        <f>SUM(B18:B19)</f>
         <v>1350</v>
       </c>
-      <c r="C17">
+      <c r="C20">
         <f>HepaticGradient</f>
         <v>6</v>
       </c>
-      <c r="D17" s="1">
-        <f>B17/C17</f>
+      <c r="D20" s="1">
+        <f>B20/C20</f>
         <v>225</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E20" s="1">
         <f>LiverMassMale</f>
         <v>1950</v>
       </c>
-      <c r="F17" s="4">
-        <f>D17/E17</f>
+      <c r="F20" s="4">
+        <f>D20/E20</f>
         <v>0.11538461538461539</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>130</v>
-      </c>
-      <c r="B19" s="1">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="1">
         <f>LiverFlowMale</f>
         <v>1350</v>
       </c>
-      <c r="C19">
+      <c r="C22">
         <f>HepaticGradient</f>
         <v>6</v>
       </c>
-      <c r="D19" s="1">
-        <f>B19/C19</f>
+      <c r="D22" s="1">
+        <f>B22/C22</f>
         <v>225</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="E22" s="1"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B24" s="1">
         <f>LHeartFlowMale</f>
         <v>179.28</v>
       </c>
-      <c r="C21">
+      <c r="C24">
         <f>CoronaryGradient</f>
         <v>95</v>
       </c>
-      <c r="D21" s="6">
-        <f>B21/C21</f>
+      <c r="D24" s="6">
+        <f>B24/C24</f>
         <v>1.8871578947368421</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E24" s="1">
         <f>LHeartMassMale</f>
         <v>292.57499999999993</v>
       </c>
-      <c r="F21" s="4">
-        <f>D21/E21</f>
+      <c r="F24" s="4">
+        <f>D24/E24</f>
         <v>6.4501679731243013E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25">
+        <f>LHeartLargeVesselGradient</f>
+        <v>3.5</v>
+      </c>
+      <c r="D25" s="5">
+        <f>LHeartFlowMale/LHeartLargeVesselGradient</f>
+        <v>51.222857142857144</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="4">
+        <f>D25/E24</f>
+        <v>0.17507598784194534</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26">
+        <f>LHeartSmallVesselGradient</f>
+        <v>91.5</v>
+      </c>
+      <c r="D26" s="6">
+        <f>LHeartFlowMale/LHeartSmallVesselGradient</f>
+        <v>1.9593442622950821</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="4">
+        <f>D26/E24</f>
+        <v>6.6968957098011879E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B27" s="1">
         <f>RHeartFlowMale</f>
         <v>36.720000000000006</v>
       </c>
-      <c r="C22">
+      <c r="C27">
         <f>CoronaryGradient</f>
         <v>95</v>
       </c>
-      <c r="D22" s="6">
-        <f>B22/C22</f>
+      <c r="D27" s="6">
+        <f>B27/C27</f>
         <v>0.38652631578947377</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E27" s="1">
         <f>RHeartMassMale</f>
         <v>59.924999999999997</v>
       </c>
-      <c r="F22" s="4">
-        <f>D22/E22</f>
+      <c r="F27" s="4">
+        <f>D27/E27</f>
         <v>6.4501679731243022E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="1">
-        <f>SUM(B21:B22)</f>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28">
+        <f>RheartLargeVesselGradient</f>
+        <v>3.5</v>
+      </c>
+      <c r="D28" s="5">
+        <f>RHeartFlowMale/RheartLargeVesselGradient</f>
+        <v>10.491428571428573</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="4">
+        <f>D28/E27</f>
+        <v>0.17507598784194531</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29">
+        <f>RHeartSmallVesselGradient</f>
+        <v>91.5</v>
+      </c>
+      <c r="D29" s="6">
+        <f>RHeartFlowMale/RHeartSmallVesselGradient</f>
+        <v>0.40131147540983614</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="4">
+        <f>D29/E27</f>
+        <v>6.696895709801187E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="1">
+        <f>SUM(B24:B27)</f>
         <v>216</v>
       </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>132</v>
-      </c>
-      <c r="B25" s="1">
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="1">
         <f>SystemicVeinOutflow+HepaticVeinOutflow+CoronarySinusOutflow</f>
         <v>5400</v>
       </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34">
         <f>VenousReturn</f>
         <v>5400</v>
       </c>
-      <c r="C27">
+      <c r="C34">
         <f>PulmArtyGradient</f>
         <v>4</v>
       </c>
-      <c r="D27" s="1">
-        <f>B27/C27</f>
+      <c r="D34" s="1">
+        <f>B34/C34</f>
         <v>1350</v>
       </c>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>106</v>
-      </c>
-      <c r="B28">
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35">
         <f>VenousReturn</f>
         <v>5400</v>
       </c>
-      <c r="C28">
+      <c r="C35">
         <f>PulmCapysGradient</f>
         <v>3</v>
       </c>
-      <c r="D28" s="1">
-        <f>B28/C28</f>
+      <c r="D35" s="1">
+        <f>B35/C35</f>
         <v>1800</v>
       </c>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>133</v>
-      </c>
-      <c r="B29">
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B36">
         <f>VenousReturn</f>
         <v>5400</v>
       </c>
-      <c r="C29">
+      <c r="C36">
         <f>PulmVeinsGradient</f>
         <v>1</v>
       </c>
-      <c r="D29" s="1">
-        <f>B29/C29</f>
+      <c r="D36" s="1">
+        <f>B36/C36</f>
         <v>5400</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4657,344 +5292,177 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D23"/>
+      <selection activeCell="A3" sqref="A3:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>9700</v>
-      </c>
-      <c r="C2">
-        <v>4.7</v>
-      </c>
-      <c r="D2" s="4">
-        <f>C2/B2</f>
-        <v>4.8453608247422681E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1300</v>
-      </c>
-      <c r="C3">
-        <v>9.1</v>
-      </c>
-      <c r="D3" s="4">
-        <f>C3/B3</f>
-        <v>7.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="1">
+        <f>BaseMassMale</f>
+        <v>26032.5</v>
+      </c>
+      <c r="C5" s="7">
+        <f>BaseFlowGMale</f>
+        <v>0.16602938634399309</v>
+      </c>
+      <c r="D5" s="1">
+        <f>C5*B5</f>
+        <v>4322.16</v>
+      </c>
+      <c r="F5" s="1">
+        <f>BaseMassFemale</f>
+        <v>20794.799999999996</v>
+      </c>
+      <c r="G5" s="7">
+        <f>BaseFlowGFemale</f>
+        <v>0.17052149722811896</v>
+      </c>
+      <c r="H5" s="1">
+        <f>G5*F5</f>
+        <v>3545.9604305592875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1">
+        <f>SMuscleMassMale</f>
+        <v>26400</v>
+      </c>
+      <c r="C6" s="7">
+        <f>SMuscleFlowGMale</f>
+        <v>3.0600000000000006E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <f>C6*B6</f>
+        <v>807.84000000000015</v>
+      </c>
+      <c r="F6" s="1">
+        <f>SMuscleMassFemale</f>
+        <v>14628.900000000001</v>
+      </c>
+      <c r="G6" s="7">
+        <f>SMuscleFlowGFemale</f>
+        <v>2.983721055176489E-2</v>
+      </c>
+      <c r="H6" s="1">
+        <f>G6*F6</f>
+        <v>436.48556944071345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>16600</v>
-      </c>
-      <c r="C4">
-        <v>2.7</v>
-      </c>
-      <c r="D4" s="4">
-        <f>C4/B4</f>
-        <v>1.6265060240963855E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>1500</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5" s="4">
-        <f>C5/B5</f>
-        <v>6.6666666666666671E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>290</v>
-      </c>
-      <c r="C6">
-        <v>13.9</v>
-      </c>
-      <c r="D6" s="4">
-        <f>C6/B6</f>
-        <v>4.7931034482758622E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7">
-        <v>600</v>
-      </c>
-      <c r="D7" s="4">
-        <f>C7/B6</f>
-        <v>2.0689655172413794</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8">
-        <v>37.299999999999997</v>
-      </c>
-      <c r="D8" s="4">
-        <f>C8/B6</f>
-        <v>0.1286206896551724</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9">
-        <v>23</v>
-      </c>
-      <c r="D9" s="4">
-        <f>C9/B6</f>
-        <v>7.9310344827586213E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>260</v>
-      </c>
-      <c r="C10">
-        <v>2.1</v>
-      </c>
-      <c r="D10" s="4">
-        <f>C10/B10</f>
-        <v>8.076923076923077E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11">
-        <v>50</v>
-      </c>
-      <c r="D11" s="4">
-        <f>C11/B10</f>
-        <v>0.19230769230769232</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D12" s="4">
-        <f>C12/B10</f>
-        <v>8.461538461538463E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>1750</v>
-      </c>
-      <c r="C13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14">
-        <v>2.8</v>
-      </c>
-      <c r="D14" s="4">
-        <f>C14/B13</f>
-        <v>1.5999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16">
-        <v>178</v>
-      </c>
-      <c r="D16" s="4">
-        <f>C16/B13</f>
-        <v>0.10171428571428572</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17">
-        <v>4100</v>
-      </c>
-      <c r="C17">
-        <v>4.2</v>
-      </c>
-      <c r="D17" s="4">
-        <f>C17/B17</f>
-        <v>1.0243902439024391E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18">
-        <v>3500</v>
-      </c>
-      <c r="C18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D18" s="4">
-        <f>C18/B18</f>
-        <v>3.1428571428571432E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19">
-        <v>50</v>
-      </c>
-      <c r="C19">
-        <v>0.39</v>
-      </c>
-      <c r="D19" s="4">
-        <f>C19/B19</f>
-        <v>7.8000000000000005E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20">
-        <v>10</v>
-      </c>
-      <c r="D20" s="4">
-        <f>C20/B19</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21">
-        <v>0.4</v>
-      </c>
-      <c r="D21" s="4">
-        <f>C21/B19</f>
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22">
-        <v>27000</v>
-      </c>
-      <c r="C22">
-        <v>7.2</v>
-      </c>
-      <c r="D22" s="4">
-        <f>C22/B22</f>
-        <v>2.6666666666666668E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23">
-        <v>2550</v>
-      </c>
-      <c r="C23">
-        <v>1.6</v>
-      </c>
-      <c r="D23" s="4">
-        <f>C23/B23</f>
-        <v>6.2745098039215688E-4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24">
-        <f>SUM(B2,B3,B5:B19,B23)</f>
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25">
-        <f>SUM(B2:B23)</f>
-        <v>68600</v>
+      <c r="B7" s="1">
+        <f>FatMassMale</f>
+        <v>16050</v>
+      </c>
+      <c r="C7" s="7">
+        <f>FatFlowGMale</f>
+        <v>1.6822429906542057E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <f>C7*B7</f>
+        <v>270</v>
+      </c>
+      <c r="F7" s="1">
+        <f>FatMassFemale</f>
+        <v>19767.150000000001</v>
+      </c>
+      <c r="G7" s="7">
+        <f>FatFlowGFemale</f>
+        <v>1.8715596330275232E-2</v>
+      </c>
+      <c r="H7" s="1">
+        <f>G7*F7</f>
+        <v>369.95400000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1">
+        <f>SUM(B5:B7)</f>
+        <v>68482.5</v>
+      </c>
+      <c r="D8" s="1">
+        <f>SUM(D5:D7)</f>
+        <v>5400</v>
+      </c>
+      <c r="F8" s="1">
+        <f>SUM(F5:F7)</f>
+        <v>55190.85</v>
+      </c>
+      <c r="H8" s="1">
+        <f>SUM(H5:H7)</f>
+        <v>4352.4000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="1">
+        <f>OrganMassMale</f>
+        <v>68482.5</v>
+      </c>
+      <c r="D9" s="1">
+        <f>CardiacOutputMale</f>
+        <v>5400</v>
+      </c>
+      <c r="F9" s="1">
+        <f>OrganMassFemale</f>
+        <v>55190.85</v>
+      </c>
+      <c r="H9" s="1">
+        <f>CardiacOutputFemale</f>
+        <v>4352.4000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HumModRepository - Pushing a current log.
</commit_message>
<xml_diff>
--- a/NormalValues/NormalValues.xlsx
+++ b/NormalValues/NormalValues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6465" tabRatio="627" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="6465" tabRatio="627" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Body Mass" sheetId="8" r:id="rId1"/>
@@ -1016,7 +1016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -4661,8 +4661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5021,7 +5021,10 @@
         <v>3.6404494382022472</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4">
+        <f>D19/E20</f>
+        <v>1.8668971477960243E-3</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">

</xml_diff>